<commit_message>
update resultados (cmc and dmft datasets, but incompleted)
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="131">
   <si>
     <t>Ferramenta</t>
   </si>
@@ -374,6 +374,48 @@
   </si>
   <si>
     <t>Melhor: 0.8421</t>
+  </si>
+  <si>
+    <t>5m24.868s</t>
+  </si>
+  <si>
+    <t>1m33.04s</t>
+  </si>
+  <si>
+    <t>5m40.270304</t>
+  </si>
+  <si>
+    <t>1m47.714s</t>
+  </si>
+  <si>
+    <t>Melhor: 0.5723</t>
+  </si>
+  <si>
+    <t>pipeline scikit learn com Random Forest</t>
+  </si>
+  <si>
+    <t>4m18s</t>
+  </si>
+  <si>
+    <t>falta fazer</t>
+  </si>
+  <si>
+    <t>Melhor: 0.2623</t>
+  </si>
+  <si>
+    <t>4m31.271s</t>
+  </si>
+  <si>
+    <t>52.16s</t>
+  </si>
+  <si>
+    <t>LightGBMClassifier</t>
+  </si>
+  <si>
+    <t>5m44.979605s</t>
+  </si>
+  <si>
+    <t>01m46.66s</t>
   </si>
 </sst>
 </file>
@@ -397,12 +439,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -480,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -555,16 +603,40 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -590,22 +662,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -890,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" topLeftCell="D61" workbookViewId="0">
+      <selection activeCell="N83" sqref="L75:N89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,10 +1021,10 @@
       </c>
     </row>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="28" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="2"/>
@@ -983,25 +1046,25 @@
       <c r="K2" s="2">
         <v>2.3615173893038102</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="L2" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="M2" s="27" t="s">
+      <c r="M2" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="N2" s="27">
+      <c r="N2" s="35">
         <v>73</v>
       </c>
-      <c r="R2" s="26" t="s">
+      <c r="R2" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="26"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="28"/>
     </row>
     <row r="3" spans="2:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="26"/>
-      <c r="D3" s="26"/>
+      <c r="B3" s="28"/>
+      <c r="D3" s="28"/>
       <c r="E3" s="2" t="s">
         <v>20</v>
       </c>
@@ -1023,9 +1086,9 @@
       <c r="K3" s="2">
         <v>2.2556710599482699</v>
       </c>
-      <c r="L3" s="30"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
       <c r="R3" s="19" t="s">
         <v>2</v>
       </c>
@@ -1040,8 +1103,8 @@
       </c>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
-      <c r="D4" s="26"/>
+      <c r="B4" s="28"/>
+      <c r="D4" s="28"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
         <v>15</v>
@@ -1061,9 +1124,9 @@
       <c r="K4" s="2">
         <v>2.2502649752898698</v>
       </c>
-      <c r="L4" s="30"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
       <c r="R4" s="19" t="s">
         <v>3</v>
       </c>
@@ -1078,8 +1141,8 @@
       </c>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="26"/>
-      <c r="D5" s="26"/>
+      <c r="B5" s="28"/>
+      <c r="D5" s="28"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
         <v>17</v>
@@ -1099,9 +1162,9 @@
       <c r="K5" s="7">
         <v>2.0563812623190301</v>
       </c>
-      <c r="L5" s="30"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
       <c r="R5" s="19" t="s">
         <v>28</v>
       </c>
@@ -1116,8 +1179,8 @@
       </c>
     </row>
     <row r="6" spans="2:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="26"/>
-      <c r="D6" s="26"/>
+      <c r="B6" s="28"/>
+      <c r="D6" s="28"/>
       <c r="E6" s="5" t="s">
         <v>36</v>
       </c>
@@ -1139,9 +1202,9 @@
       <c r="K6" s="4">
         <v>2.5263518439219701</v>
       </c>
-      <c r="L6" s="30"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
       <c r="R6" s="19" t="s">
         <v>38</v>
       </c>
@@ -1156,8 +1219,8 @@
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="26"/>
-      <c r="D7" s="26"/>
+      <c r="B7" s="28"/>
+      <c r="D7" s="28"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
         <v>23</v>
@@ -1177,9 +1240,9 @@
       <c r="K7" s="2">
         <v>2.29</v>
       </c>
-      <c r="L7" s="30"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
       <c r="R7" s="19" t="s">
         <v>44</v>
       </c>
@@ -1194,8 +1257,8 @@
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="26"/>
-      <c r="D8" s="26"/>
+      <c r="B8" s="28"/>
+      <c r="D8" s="28"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
         <v>25</v>
@@ -1215,9 +1278,9 @@
       <c r="K8" s="4">
         <v>2.0925560658435201</v>
       </c>
-      <c r="L8" s="30"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
       <c r="R8" s="19" t="s">
         <v>50</v>
       </c>
@@ -1232,8 +1295,8 @@
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="26"/>
-      <c r="D9" s="39"/>
+      <c r="B9" s="28"/>
+      <c r="D9" s="31"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8" t="s">
         <v>26</v>
@@ -1245,9 +1308,9 @@
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="35"/>
       <c r="R9" s="19" t="s">
         <v>57</v>
       </c>
@@ -1262,7 +1325,7 @@
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="26"/>
+      <c r="B10" s="28"/>
       <c r="D10" s="12"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
@@ -1288,8 +1351,8 @@
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="26"/>
-      <c r="D11" s="37" t="s">
+      <c r="B11" s="28"/>
+      <c r="D11" s="32" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="9" t="s">
@@ -1313,13 +1376,13 @@
       <c r="K11" s="16">
         <v>42.172544929804403</v>
       </c>
-      <c r="L11" s="32" t="s">
+      <c r="L11" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="M11" s="41" t="s">
+      <c r="M11" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="N11" s="41">
+      <c r="N11" s="36">
         <v>160</v>
       </c>
       <c r="R11" s="19" t="s">
@@ -1336,8 +1399,8 @@
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="26"/>
-      <c r="D12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="D12" s="33"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
         <v>15</v>
@@ -1357,9 +1420,9 @@
       <c r="K12" s="4">
         <v>42.4696075892439</v>
       </c>
-      <c r="L12" s="33"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
       <c r="R12" s="19" t="s">
         <v>103</v>
       </c>
@@ -1374,8 +1437,8 @@
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="26"/>
-      <c r="D13" s="28"/>
+      <c r="B13" s="28"/>
+      <c r="D13" s="33"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
         <v>17</v>
@@ -1395,9 +1458,9 @@
       <c r="K13" s="4">
         <v>43.043253511127602</v>
       </c>
-      <c r="L13" s="33"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
       <c r="R13" s="20" t="s">
         <v>108</v>
       </c>
@@ -1412,8 +1475,8 @@
       </c>
     </row>
     <row r="14" spans="2:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="26"/>
-      <c r="D14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="D14" s="33"/>
       <c r="E14" s="5" t="s">
         <v>36</v>
       </c>
@@ -1435,9 +1498,9 @@
       <c r="K14" s="4">
         <v>42.455950916767499</v>
       </c>
-      <c r="L14" s="33"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
       <c r="R14" s="20" t="s">
         <v>109</v>
       </c>
@@ -1452,8 +1515,8 @@
       </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B15" s="26"/>
-      <c r="D15" s="28"/>
+      <c r="B15" s="28"/>
+      <c r="D15" s="33"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4" t="s">
         <v>23</v>
@@ -1473,9 +1536,9 @@
       <c r="K15" s="4">
         <v>42.61</v>
       </c>
-      <c r="L15" s="33"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="41"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
       <c r="R15" s="20" t="s">
         <v>110</v>
       </c>
@@ -1490,8 +1553,8 @@
       </c>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B16" s="26"/>
-      <c r="D16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="D16" s="33"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
         <v>25</v>
@@ -1511,13 +1574,13 @@
       <c r="K16" s="4">
         <v>42.954693127434403</v>
       </c>
-      <c r="L16" s="33"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="41"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="26"/>
-      <c r="D17" s="40"/>
+      <c r="B17" s="28"/>
+      <c r="D17" s="34"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8" t="s">
         <v>26</v>
@@ -1529,12 +1592,12 @@
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="41"/>
-      <c r="N17" s="41"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="26"/>
+      <c r="B18" s="28"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
@@ -1548,8 +1611,8 @@
       <c r="N18" s="11"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="26"/>
-      <c r="D19" s="37" t="s">
+      <c r="B19" s="28"/>
+      <c r="D19" s="32" t="s">
         <v>38</v>
       </c>
       <c r="E19" s="9" t="s">
@@ -1573,19 +1636,19 @@
       <c r="K19" s="9">
         <v>0.23469975874427401</v>
       </c>
-      <c r="L19" s="35" t="s">
+      <c r="L19" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="M19" s="25" t="s">
+      <c r="M19" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="N19" s="25">
+      <c r="N19" s="29">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="26"/>
-      <c r="D20" s="28"/>
+      <c r="B20" s="28"/>
+      <c r="D20" s="33"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
         <v>15</v>
@@ -1605,13 +1668,13 @@
       <c r="K20" s="4">
         <v>0.26615681314328199</v>
       </c>
-      <c r="L20" s="36"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="25"/>
+      <c r="L20" s="44"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="26"/>
-      <c r="D21" s="28"/>
+      <c r="B21" s="28"/>
+      <c r="D21" s="33"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
         <v>17</v>
@@ -1631,13 +1694,13 @@
       <c r="K21" s="4">
         <v>0.27054514227366</v>
       </c>
-      <c r="L21" s="36"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="25"/>
+      <c r="L21" s="44"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
     </row>
     <row r="22" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="26"/>
-      <c r="D22" s="28"/>
+      <c r="B22" s="28"/>
+      <c r="D22" s="33"/>
       <c r="E22" s="5" t="s">
         <v>36</v>
       </c>
@@ -1659,13 +1722,13 @@
       <c r="K22" s="7">
         <v>0.23440350034482499</v>
       </c>
-      <c r="L22" s="36"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="25"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="26"/>
-      <c r="D23" s="28"/>
+      <c r="B23" s="28"/>
+      <c r="D23" s="33"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4" t="s">
         <v>23</v>
@@ -1685,13 +1748,13 @@
       <c r="K23" s="4">
         <v>0.27</v>
       </c>
-      <c r="L23" s="36"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="26"/>
-      <c r="D24" s="28"/>
+      <c r="B24" s="28"/>
+      <c r="D24" s="33"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4" t="s">
         <v>25</v>
@@ -1711,13 +1774,13 @@
       <c r="K24" s="4">
         <v>0.24189871737548899</v>
       </c>
-      <c r="L24" s="36"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="25"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="26"/>
-      <c r="D25" s="40"/>
+      <c r="B25" s="28"/>
+      <c r="D25" s="34"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8" t="s">
         <v>26</v>
@@ -1729,12 +1792,12 @@
       </c>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
-      <c r="L25" s="37"/>
-      <c r="M25" s="25"/>
-      <c r="N25" s="25"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="26"/>
+      <c r="B26" s="28"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
@@ -1748,8 +1811,8 @@
       <c r="N26" s="11"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="26"/>
-      <c r="D27" s="37" t="s">
+      <c r="B27" s="28"/>
+      <c r="D27" s="32" t="s">
         <v>45</v>
       </c>
       <c r="E27" s="9" t="s">
@@ -1773,19 +1836,19 @@
       <c r="K27" s="9">
         <v>141.96334027640401</v>
       </c>
-      <c r="L27" s="35" t="s">
+      <c r="L27" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="M27" s="25" t="s">
+      <c r="M27" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="N27" s="25">
+      <c r="N27" s="29">
         <v>15</v>
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="26"/>
-      <c r="D28" s="28"/>
+      <c r="B28" s="28"/>
+      <c r="D28" s="33"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4" t="s">
         <v>15</v>
@@ -1805,13 +1868,13 @@
       <c r="K28" s="4">
         <v>146.72373452591</v>
       </c>
-      <c r="L28" s="36"/>
-      <c r="M28" s="25"/>
-      <c r="N28" s="25"/>
+      <c r="L28" s="44"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="29"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="26"/>
-      <c r="D29" s="28"/>
+      <c r="B29" s="28"/>
+      <c r="D29" s="33"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4" t="s">
         <v>17</v>
@@ -1831,13 +1894,13 @@
       <c r="K29" s="7">
         <v>140.69022615456799</v>
       </c>
-      <c r="L29" s="36"/>
-      <c r="M29" s="25"/>
-      <c r="N29" s="25"/>
+      <c r="L29" s="44"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="29"/>
     </row>
     <row r="30" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B30" s="26"/>
-      <c r="D30" s="28"/>
+      <c r="B30" s="28"/>
+      <c r="D30" s="33"/>
       <c r="E30" s="5" t="s">
         <v>36</v>
       </c>
@@ -1859,13 +1922,13 @@
       <c r="K30" s="4">
         <v>142.52852874723999</v>
       </c>
-      <c r="L30" s="36"/>
-      <c r="M30" s="25"/>
-      <c r="N30" s="25"/>
+      <c r="L30" s="44"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="29"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="26"/>
-      <c r="D31" s="28"/>
+      <c r="B31" s="28"/>
+      <c r="D31" s="33"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4" t="s">
         <v>23</v>
@@ -1885,13 +1948,13 @@
       <c r="K31" s="4">
         <v>152.29</v>
       </c>
-      <c r="L31" s="36"/>
-      <c r="M31" s="25"/>
-      <c r="N31" s="25"/>
+      <c r="L31" s="44"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="29"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B32" s="26"/>
-      <c r="D32" s="28"/>
+      <c r="B32" s="28"/>
+      <c r="D32" s="33"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4" t="s">
         <v>25</v>
@@ -1911,13 +1974,13 @@
       <c r="K32" s="4">
         <v>144.833568734441</v>
       </c>
-      <c r="L32" s="36"/>
-      <c r="M32" s="25"/>
-      <c r="N32" s="25"/>
+      <c r="L32" s="44"/>
+      <c r="M32" s="29"/>
+      <c r="N32" s="29"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="26"/>
-      <c r="D33" s="40"/>
+      <c r="B33" s="28"/>
+      <c r="D33" s="34"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8" t="s">
         <v>26</v>
@@ -1929,9 +1992,9 @@
       </c>
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="25"/>
-      <c r="N33" s="25"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="29"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D34" s="13"/>
@@ -1947,10 +2010,10 @@
       <c r="N34" s="11"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="38" t="s">
+      <c r="D35" s="30" t="s">
         <v>50</v>
       </c>
       <c r="E35" s="9" t="s">
@@ -1974,19 +2037,19 @@
       <c r="K35" s="9">
         <v>0.910468209203948</v>
       </c>
-      <c r="L35" s="35" t="s">
+      <c r="L35" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="M35" s="25" t="s">
+      <c r="M35" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="N35" s="25">
+      <c r="N35" s="29">
         <v>5132</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B36" s="27"/>
-      <c r="D36" s="26"/>
+      <c r="B36" s="35"/>
+      <c r="D36" s="28"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4" t="s">
         <v>15</v>
@@ -2006,13 +2069,13 @@
       <c r="K36" s="4">
         <v>0.88615775755244997</v>
       </c>
-      <c r="L36" s="36"/>
-      <c r="M36" s="25"/>
-      <c r="N36" s="25"/>
+      <c r="L36" s="44"/>
+      <c r="M36" s="29"/>
+      <c r="N36" s="29"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="27"/>
-      <c r="D37" s="26"/>
+      <c r="B37" s="35"/>
+      <c r="D37" s="28"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4" t="s">
         <v>17</v>
@@ -2032,13 +2095,13 @@
       <c r="K37" s="4">
         <v>0.87077511430158505</v>
       </c>
-      <c r="L37" s="36"/>
-      <c r="M37" s="25"/>
-      <c r="N37" s="25"/>
+      <c r="L37" s="44"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
     </row>
     <row r="38" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B38" s="27"/>
-      <c r="D38" s="26"/>
+      <c r="B38" s="35"/>
+      <c r="D38" s="28"/>
       <c r="E38" s="5" t="s">
         <v>36</v>
       </c>
@@ -2060,13 +2123,13 @@
       <c r="K38" s="4">
         <v>0.91063111566893096</v>
       </c>
-      <c r="L38" s="36"/>
-      <c r="M38" s="25"/>
-      <c r="N38" s="25"/>
+      <c r="L38" s="44"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B39" s="27"/>
-      <c r="D39" s="26"/>
+      <c r="B39" s="35"/>
+      <c r="D39" s="28"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4" t="s">
         <v>23</v>
@@ -2086,13 +2149,13 @@
       <c r="K39" s="4">
         <v>0.91</v>
       </c>
-      <c r="L39" s="36"/>
-      <c r="M39" s="25"/>
-      <c r="N39" s="25"/>
+      <c r="L39" s="44"/>
+      <c r="M39" s="29"/>
+      <c r="N39" s="29"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B40" s="27"/>
-      <c r="D40" s="26"/>
+      <c r="B40" s="35"/>
+      <c r="D40" s="28"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4" t="s">
         <v>25</v>
@@ -2112,13 +2175,13 @@
       <c r="K40" s="7">
         <v>0.91188896722642299</v>
       </c>
-      <c r="L40" s="36"/>
-      <c r="M40" s="25"/>
-      <c r="N40" s="25"/>
+      <c r="L40" s="44"/>
+      <c r="M40" s="29"/>
+      <c r="N40" s="29"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B41" s="27"/>
-      <c r="D41" s="39"/>
+      <c r="B41" s="35"/>
+      <c r="D41" s="31"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8" t="s">
         <v>26</v>
@@ -2130,12 +2193,12 @@
       </c>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
-      <c r="L41" s="37"/>
-      <c r="M41" s="25"/>
-      <c r="N41" s="25"/>
+      <c r="L41" s="32"/>
+      <c r="M41" s="29"/>
+      <c r="N41" s="29"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B42" s="27"/>
+      <c r="B42" s="35"/>
       <c r="D42" s="12"/>
       <c r="E42" s="13"/>
       <c r="F42" s="13"/>
@@ -2149,8 +2212,8 @@
       <c r="N42" s="11"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B43" s="27"/>
-      <c r="D43" s="38" t="s">
+      <c r="B43" s="35"/>
+      <c r="D43" s="30" t="s">
         <v>57</v>
       </c>
       <c r="E43" s="9" t="s">
@@ -2174,19 +2237,19 @@
       <c r="K43" s="9">
         <v>0.78503433208489304</v>
       </c>
-      <c r="L43" s="25" t="s">
+      <c r="L43" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="M43" s="25" t="s">
+      <c r="M43" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="N43" s="25">
+      <c r="N43" s="29">
         <v>419021</v>
       </c>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B44" s="27"/>
-      <c r="D44" s="26"/>
+      <c r="B44" s="35"/>
+      <c r="D44" s="28"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4" t="s">
         <v>15</v>
@@ -2206,13 +2269,13 @@
       <c r="K44" s="4">
         <v>0.59706616729088602</v>
       </c>
-      <c r="L44" s="28"/>
-      <c r="M44" s="25"/>
-      <c r="N44" s="25"/>
+      <c r="L44" s="33"/>
+      <c r="M44" s="29"/>
+      <c r="N44" s="29"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B45" s="27"/>
-      <c r="D45" s="26"/>
+      <c r="B45" s="35"/>
+      <c r="D45" s="28"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4" t="s">
         <v>17</v>
@@ -2232,13 +2295,13 @@
       <c r="K45" s="4">
         <v>0.71168851435705305</v>
       </c>
-      <c r="L45" s="28"/>
-      <c r="M45" s="25"/>
-      <c r="N45" s="25"/>
+      <c r="L45" s="33"/>
+      <c r="M45" s="29"/>
+      <c r="N45" s="29"/>
     </row>
     <row r="46" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B46" s="27"/>
-      <c r="D46" s="26"/>
+      <c r="B46" s="35"/>
+      <c r="D46" s="28"/>
       <c r="E46" s="5" t="s">
         <v>36</v>
       </c>
@@ -2260,13 +2323,13 @@
       <c r="K46" s="4">
         <v>0.77699750312109805</v>
       </c>
-      <c r="L46" s="28"/>
-      <c r="M46" s="25"/>
-      <c r="N46" s="25"/>
+      <c r="L46" s="33"/>
+      <c r="M46" s="29"/>
+      <c r="N46" s="29"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B47" s="27"/>
-      <c r="D47" s="26"/>
+      <c r="B47" s="35"/>
+      <c r="D47" s="28"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4" t="s">
         <v>23</v>
@@ -2286,13 +2349,13 @@
       <c r="K47" s="7">
         <v>0.8</v>
       </c>
-      <c r="L47" s="28"/>
-      <c r="M47" s="25"/>
-      <c r="N47" s="25"/>
+      <c r="L47" s="33"/>
+      <c r="M47" s="29"/>
+      <c r="N47" s="29"/>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B48" s="27"/>
-      <c r="D48" s="26"/>
+      <c r="B48" s="35"/>
+      <c r="D48" s="28"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4" t="s">
         <v>25</v>
@@ -2312,13 +2375,13 @@
       <c r="K48" s="7">
         <v>0.80024968789013695</v>
       </c>
-      <c r="L48" s="28"/>
-      <c r="M48" s="25"/>
-      <c r="N48" s="25"/>
+      <c r="L48" s="33"/>
+      <c r="M48" s="29"/>
+      <c r="N48" s="29"/>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B49" s="27"/>
-      <c r="D49" s="39"/>
+      <c r="B49" s="35"/>
+      <c r="D49" s="31"/>
       <c r="E49" s="8"/>
       <c r="F49" s="8" t="s">
         <v>26</v>
@@ -2330,12 +2393,12 @@
       </c>
       <c r="J49" s="8"/>
       <c r="K49" s="8"/>
-      <c r="L49" s="28"/>
-      <c r="M49" s="25"/>
-      <c r="N49" s="25"/>
+      <c r="L49" s="33"/>
+      <c r="M49" s="29"/>
+      <c r="N49" s="29"/>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B50" s="27"/>
+      <c r="B50" s="35"/>
       <c r="D50" s="12"/>
       <c r="E50" s="13"/>
       <c r="F50" s="13"/>
@@ -2349,8 +2412,8 @@
       <c r="N50" s="11"/>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B51" s="27"/>
-      <c r="D51" s="38" t="s">
+      <c r="B51" s="35"/>
+      <c r="D51" s="30" t="s">
         <v>62</v>
       </c>
       <c r="E51" s="9" t="s">
@@ -2374,19 +2437,19 @@
       <c r="K51" s="9">
         <v>0.94655497110201903</v>
       </c>
-      <c r="L51" s="25" t="s">
+      <c r="L51" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="M51" s="25" t="s">
+      <c r="M51" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="N51" s="25">
+      <c r="N51" s="29">
         <v>147659</v>
       </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B52" s="27"/>
-      <c r="D52" s="26"/>
+      <c r="B52" s="35"/>
+      <c r="D52" s="28"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4" t="s">
         <v>15</v>
@@ -2406,13 +2469,13 @@
       <c r="K52" s="4">
         <v>0.83995714007403</v>
       </c>
-      <c r="L52" s="28"/>
-      <c r="M52" s="25"/>
-      <c r="N52" s="25"/>
+      <c r="L52" s="33"/>
+      <c r="M52" s="29"/>
+      <c r="N52" s="29"/>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B53" s="27"/>
-      <c r="D53" s="26"/>
+      <c r="B53" s="35"/>
+      <c r="D53" s="28"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4" t="s">
         <v>17</v>
@@ -2432,13 +2495,13 @@
       <c r="K53" s="7">
         <v>1</v>
       </c>
-      <c r="L53" s="28"/>
-      <c r="M53" s="25"/>
-      <c r="N53" s="25"/>
+      <c r="L53" s="33"/>
+      <c r="M53" s="29"/>
+      <c r="N53" s="29"/>
     </row>
     <row r="54" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B54" s="27"/>
-      <c r="D54" s="26"/>
+      <c r="B54" s="35"/>
+      <c r="D54" s="28"/>
       <c r="E54" s="5" t="s">
         <v>36</v>
       </c>
@@ -2460,13 +2523,13 @@
       <c r="K54" s="4">
         <v>0.97873848082154702</v>
       </c>
-      <c r="L54" s="28"/>
-      <c r="M54" s="25"/>
-      <c r="N54" s="25"/>
+      <c r="L54" s="33"/>
+      <c r="M54" s="29"/>
+      <c r="N54" s="29"/>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B55" s="27"/>
-      <c r="D55" s="26"/>
+      <c r="B55" s="35"/>
+      <c r="D55" s="28"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4" t="s">
         <v>23</v>
@@ -2486,13 +2549,13 @@
       <c r="K55" s="4">
         <v>0.94</v>
       </c>
-      <c r="L55" s="28"/>
-      <c r="M55" s="25"/>
-      <c r="N55" s="25"/>
+      <c r="L55" s="33"/>
+      <c r="M55" s="29"/>
+      <c r="N55" s="29"/>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B56" s="27"/>
-      <c r="D56" s="26"/>
+      <c r="B56" s="35"/>
+      <c r="D56" s="28"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4" t="s">
         <v>25</v>
@@ -2512,13 +2575,13 @@
       <c r="K56" s="7">
         <v>1</v>
       </c>
-      <c r="L56" s="28"/>
-      <c r="M56" s="25"/>
-      <c r="N56" s="25"/>
+      <c r="L56" s="33"/>
+      <c r="M56" s="29"/>
+      <c r="N56" s="29"/>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B57" s="27"/>
-      <c r="D57" s="39"/>
+      <c r="B57" s="35"/>
+      <c r="D57" s="31"/>
       <c r="E57" s="8"/>
       <c r="F57" s="8" t="s">
         <v>26</v>
@@ -2530,12 +2593,12 @@
       </c>
       <c r="J57" s="8"/>
       <c r="K57" s="8"/>
-      <c r="L57" s="28"/>
-      <c r="M57" s="25"/>
-      <c r="N57" s="25"/>
+      <c r="L57" s="33"/>
+      <c r="M57" s="29"/>
+      <c r="N57" s="29"/>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B58" s="27"/>
+      <c r="B58" s="35"/>
       <c r="D58" s="12"/>
       <c r="E58" s="13"/>
       <c r="F58" s="13"/>
@@ -2549,8 +2612,8 @@
       <c r="N58" s="11"/>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B59" s="27"/>
-      <c r="D59" s="26" t="s">
+      <c r="B59" s="35"/>
+      <c r="D59" s="28" t="s">
         <v>103</v>
       </c>
       <c r="E59" s="18" t="s">
@@ -2568,30 +2631,30 @@
       <c r="I59" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="J59" s="42">
+      <c r="J59" s="27">
         <v>0.84142862855390999</v>
       </c>
-      <c r="K59" s="42">
+      <c r="K59" s="27">
         <v>0.80959113938965399</v>
       </c>
-      <c r="L59" s="25" t="s">
+      <c r="L59" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="M59" s="25" t="s">
+      <c r="M59" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="N59" s="25">
+      <c r="N59" s="29">
         <v>132164</v>
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B60" s="27"/>
-      <c r="D60" s="26"/>
+      <c r="B60" s="35"/>
+      <c r="D60" s="28"/>
       <c r="E60" s="18"/>
       <c r="F60" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G60" s="42" t="s">
+      <c r="G60" s="27" t="s">
         <v>113</v>
       </c>
       <c r="H60" s="22" t="s">
@@ -2600,19 +2663,19 @@
       <c r="I60" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="J60" s="42">
+      <c r="J60" s="27">
         <v>0.85749699999999995</v>
       </c>
-      <c r="K60" s="42">
+      <c r="K60" s="27">
         <v>0.72940968540120099</v>
       </c>
-      <c r="L60" s="25"/>
-      <c r="M60" s="25"/>
-      <c r="N60" s="25"/>
+      <c r="L60" s="29"/>
+      <c r="M60" s="29"/>
+      <c r="N60" s="29"/>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B61" s="27"/>
-      <c r="D61" s="26"/>
+      <c r="B61" s="35"/>
+      <c r="D61" s="28"/>
       <c r="E61" s="18"/>
       <c r="F61" s="18" t="s">
         <v>17</v>
@@ -2626,26 +2689,26 @@
       <c r="I61" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="J61" s="42">
+      <c r="J61" s="27">
         <v>0.848912</v>
       </c>
-      <c r="K61" s="42">
+      <c r="K61" s="27">
         <v>0.65676917638741605</v>
       </c>
-      <c r="L61" s="25"/>
-      <c r="M61" s="25"/>
-      <c r="N61" s="25"/>
+      <c r="L61" s="29"/>
+      <c r="M61" s="29"/>
+      <c r="N61" s="29"/>
     </row>
     <row r="62" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B62" s="27"/>
-      <c r="D62" s="26"/>
+      <c r="B62" s="35"/>
+      <c r="D62" s="28"/>
       <c r="E62" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F62" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G62" s="42" t="s">
+      <c r="G62" s="27" t="s">
         <v>114</v>
       </c>
       <c r="H62" s="22" t="s">
@@ -2657,21 +2720,21 @@
       <c r="J62" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="K62" s="42">
+      <c r="K62" s="27">
         <v>0.81654294803817595</v>
       </c>
-      <c r="L62" s="25"/>
-      <c r="M62" s="25"/>
-      <c r="N62" s="25"/>
+      <c r="L62" s="29"/>
+      <c r="M62" s="29"/>
+      <c r="N62" s="29"/>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B63" s="27"/>
-      <c r="D63" s="26"/>
+      <c r="B63" s="35"/>
+      <c r="D63" s="28"/>
       <c r="E63" s="18"/>
       <c r="F63" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G63" s="42" t="s">
+      <c r="G63" s="27" t="s">
         <v>111</v>
       </c>
       <c r="H63" s="22" t="s">
@@ -2680,24 +2743,24 @@
       <c r="I63" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="J63" s="42">
+      <c r="J63" s="27">
         <v>1</v>
       </c>
-      <c r="K63" s="42">
+      <c r="K63" s="27">
         <v>0.81</v>
       </c>
-      <c r="L63" s="25"/>
-      <c r="M63" s="25"/>
-      <c r="N63" s="25"/>
+      <c r="L63" s="29"/>
+      <c r="M63" s="29"/>
+      <c r="N63" s="29"/>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B64" s="27"/>
-      <c r="D64" s="26"/>
+      <c r="B64" s="35"/>
+      <c r="D64" s="28"/>
       <c r="E64" s="18"/>
       <c r="F64" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G64" s="42" t="s">
+      <c r="G64" s="27" t="s">
         <v>115</v>
       </c>
       <c r="H64" s="22" t="s">
@@ -2706,39 +2769,39 @@
       <c r="I64" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="J64" s="42">
+      <c r="J64" s="27">
         <v>0.76869806094182802</v>
       </c>
-      <c r="K64" s="42">
+      <c r="K64" s="27">
         <v>0.80452456698480002</v>
       </c>
-      <c r="L64" s="25"/>
-      <c r="M64" s="25"/>
-      <c r="N64" s="25"/>
+      <c r="L64" s="29"/>
+      <c r="M64" s="29"/>
+      <c r="N64" s="29"/>
     </row>
     <row r="65" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B65" s="27"/>
-      <c r="D65" s="26"/>
+      <c r="B65" s="35"/>
+      <c r="D65" s="28"/>
       <c r="E65" s="18"/>
       <c r="F65" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="G65" s="42"/>
+      <c r="G65" s="27"/>
       <c r="H65" s="18"/>
       <c r="I65" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="J65" s="42"/>
-      <c r="K65" s="42"/>
-      <c r="L65" s="25"/>
-      <c r="M65" s="25"/>
-      <c r="N65" s="25"/>
+      <c r="J65" s="27"/>
+      <c r="K65" s="27"/>
+      <c r="L65" s="29"/>
+      <c r="M65" s="29"/>
+      <c r="N65" s="29"/>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B67" s="27" t="s">
+      <c r="B67" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="D67" s="26" t="s">
+      <c r="D67" s="28" t="s">
         <v>69</v>
       </c>
       <c r="E67" s="18" t="s">
@@ -2762,19 +2825,19 @@
       <c r="K67" s="18">
         <v>0.81557623894257503</v>
       </c>
-      <c r="L67" s="25" t="s">
+      <c r="L67" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="M67" s="25" t="s">
+      <c r="M67" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="N67" s="25">
+      <c r="N67" s="29">
         <v>23532</v>
       </c>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B68" s="27"/>
-      <c r="D68" s="26"/>
+      <c r="B68" s="35"/>
+      <c r="D68" s="28"/>
       <c r="E68" s="18"/>
       <c r="F68" s="18" t="s">
         <v>15</v>
@@ -2794,13 +2857,13 @@
       <c r="K68" s="18">
         <v>0.88222010940682705</v>
       </c>
-      <c r="L68" s="25"/>
-      <c r="M68" s="25"/>
-      <c r="N68" s="25"/>
+      <c r="L68" s="29"/>
+      <c r="M68" s="29"/>
+      <c r="N68" s="29"/>
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B69" s="27"/>
-      <c r="D69" s="26"/>
+      <c r="B69" s="35"/>
+      <c r="D69" s="28"/>
       <c r="E69" s="18"/>
       <c r="F69" s="18" t="s">
         <v>17</v>
@@ -2820,13 +2883,13 @@
       <c r="K69" s="18">
         <v>0.84568164621720798</v>
       </c>
-      <c r="L69" s="25"/>
-      <c r="M69" s="25"/>
-      <c r="N69" s="25"/>
+      <c r="L69" s="29"/>
+      <c r="M69" s="29"/>
+      <c r="N69" s="29"/>
     </row>
     <row r="70" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B70" s="27"/>
-      <c r="D70" s="26"/>
+      <c r="B70" s="35"/>
+      <c r="D70" s="28"/>
       <c r="E70" s="17" t="s">
         <v>36</v>
       </c>
@@ -2848,13 +2911,13 @@
       <c r="K70" s="18">
         <v>0.80867398669225798</v>
       </c>
-      <c r="L70" s="25"/>
-      <c r="M70" s="25"/>
-      <c r="N70" s="25"/>
+      <c r="L70" s="29"/>
+      <c r="M70" s="29"/>
+      <c r="N70" s="29"/>
     </row>
     <row r="71" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B71" s="27"/>
-      <c r="D71" s="26"/>
+      <c r="B71" s="35"/>
+      <c r="D71" s="28"/>
       <c r="E71" s="18"/>
       <c r="F71" s="18" t="s">
         <v>23</v>
@@ -2874,13 +2937,13 @@
       <c r="K71" s="7">
         <v>1</v>
       </c>
-      <c r="L71" s="25"/>
-      <c r="M71" s="25"/>
-      <c r="N71" s="25"/>
+      <c r="L71" s="29"/>
+      <c r="M71" s="29"/>
+      <c r="N71" s="29"/>
     </row>
     <row r="72" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B72" s="27"/>
-      <c r="D72" s="26"/>
+      <c r="B72" s="35"/>
+      <c r="D72" s="28"/>
       <c r="E72" s="18"/>
       <c r="F72" s="18" t="s">
         <v>25</v>
@@ -2900,13 +2963,13 @@
       <c r="K72" s="18">
         <v>0.75754008756888402</v>
       </c>
-      <c r="L72" s="25"/>
-      <c r="M72" s="25"/>
-      <c r="N72" s="25"/>
+      <c r="L72" s="29"/>
+      <c r="M72" s="29"/>
+      <c r="N72" s="29"/>
     </row>
     <row r="73" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B73" s="27"/>
-      <c r="D73" s="26"/>
+      <c r="B73" s="35"/>
+      <c r="D73" s="28"/>
       <c r="E73" s="18"/>
       <c r="F73" s="18" t="s">
         <v>26</v>
@@ -2918,16 +2981,16 @@
       </c>
       <c r="J73" s="18"/>
       <c r="K73" s="18"/>
-      <c r="L73" s="25"/>
-      <c r="M73" s="25"/>
-      <c r="N73" s="25"/>
+      <c r="L73" s="29"/>
+      <c r="M73" s="29"/>
+      <c r="N73" s="29"/>
     </row>
     <row r="74" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B74" s="27"/>
+      <c r="B74" s="35"/>
     </row>
     <row r="75" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B75" s="27"/>
-      <c r="D75" s="26" t="s">
+      <c r="B75" s="35"/>
+      <c r="D75" s="28" t="s">
         <v>108</v>
       </c>
       <c r="E75" s="18" t="s">
@@ -2936,119 +2999,181 @@
       <c r="F75" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G75" s="21"/>
-      <c r="H75" s="18"/>
-      <c r="I75" s="18"/>
-      <c r="J75" s="18"/>
-      <c r="K75" s="18"/>
-      <c r="L75" s="25"/>
-      <c r="M75" s="25"/>
-      <c r="N75" s="25"/>
+      <c r="G75" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="H75" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I75" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J75" s="27">
+        <v>0.51988444963277003</v>
+      </c>
+      <c r="K75" s="27">
+        <v>0.55025061075102</v>
+      </c>
+      <c r="L75" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="M75" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="N75" s="29">
+        <v>21446</v>
+      </c>
     </row>
     <row r="76" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B76" s="27"/>
-      <c r="D76" s="26"/>
+      <c r="B76" s="35"/>
+      <c r="D76" s="28"/>
       <c r="E76" s="18"/>
       <c r="F76" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G76" s="7"/>
-      <c r="H76" s="18"/>
-      <c r="I76" s="18"/>
-      <c r="J76" s="18"/>
-      <c r="K76" s="18"/>
-      <c r="L76" s="25"/>
-      <c r="M76" s="25"/>
-      <c r="N76" s="25"/>
+      <c r="G76" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H76" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="I76" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J76" s="27">
+        <v>0.54688300000000001</v>
+      </c>
+      <c r="K76" s="27">
+        <v>0.55299548558353595</v>
+      </c>
+      <c r="L76" s="29"/>
+      <c r="M76" s="29"/>
+      <c r="N76" s="29"/>
     </row>
     <row r="77" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B77" s="27"/>
-      <c r="D77" s="26"/>
+      <c r="B77" s="35"/>
+      <c r="D77" s="28"/>
       <c r="E77" s="18"/>
       <c r="F77" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G77" s="18"/>
-      <c r="H77" s="18"/>
-      <c r="I77" s="18"/>
-      <c r="J77" s="18"/>
-      <c r="K77" s="18"/>
-      <c r="L77" s="25"/>
-      <c r="M77" s="25"/>
-      <c r="N77" s="25"/>
+      <c r="G77" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="H77" s="47"/>
+      <c r="I77" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="J77" s="46"/>
+      <c r="K77" s="46"/>
+      <c r="L77" s="29"/>
+      <c r="M77" s="29"/>
+      <c r="N77" s="29"/>
     </row>
     <row r="78" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B78" s="27"/>
-      <c r="D78" s="26"/>
+      <c r="B78" s="35"/>
+      <c r="D78" s="28"/>
       <c r="E78" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F78" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G78" s="18"/>
-      <c r="H78" s="18"/>
-      <c r="I78" s="18"/>
-      <c r="J78" s="18"/>
-      <c r="K78" s="18"/>
-      <c r="L78" s="25"/>
-      <c r="M78" s="25"/>
-      <c r="N78" s="25"/>
+      <c r="G78" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="H78" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I78" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J78" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="K78" s="27">
+        <v>0.52849268592134702</v>
+      </c>
+      <c r="L78" s="29"/>
+      <c r="M78" s="29"/>
+      <c r="N78" s="29"/>
     </row>
     <row r="79" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B79" s="27"/>
-      <c r="D79" s="26"/>
+      <c r="B79" s="35"/>
+      <c r="D79" s="28"/>
       <c r="E79" s="18"/>
       <c r="F79" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G79" s="18"/>
-      <c r="H79" s="18"/>
-      <c r="I79" s="18"/>
-      <c r="J79" s="18"/>
-      <c r="K79" s="7"/>
-      <c r="L79" s="25"/>
-      <c r="M79" s="25"/>
-      <c r="N79" s="25"/>
+      <c r="G79" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="H79" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I79" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J79" s="27">
+        <v>0.91148499999999999</v>
+      </c>
+      <c r="K79" s="27">
+        <v>0.49690000000000001</v>
+      </c>
+      <c r="L79" s="29"/>
+      <c r="M79" s="29"/>
+      <c r="N79" s="29"/>
     </row>
     <row r="80" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B80" s="27"/>
-      <c r="D80" s="26"/>
+      <c r="B80" s="35"/>
+      <c r="D80" s="28"/>
       <c r="E80" s="18"/>
       <c r="F80" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G80" s="18"/>
-      <c r="H80" s="18"/>
-      <c r="I80" s="18"/>
-      <c r="J80" s="18"/>
-      <c r="K80" s="18"/>
-      <c r="L80" s="25"/>
-      <c r="M80" s="25"/>
-      <c r="N80" s="25"/>
+      <c r="G80" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="H80" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="I80" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J80" s="27">
+        <v>0.52831990442326004</v>
+      </c>
+      <c r="K80" s="27">
+        <v>0.56739713139489401</v>
+      </c>
+      <c r="L80" s="29"/>
+      <c r="M80" s="29"/>
+      <c r="N80" s="29"/>
     </row>
     <row r="81" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B81" s="27"/>
-      <c r="D81" s="26"/>
+      <c r="B81" s="35"/>
+      <c r="D81" s="28"/>
       <c r="E81" s="18"/>
       <c r="F81" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="G81" s="18"/>
+      <c r="G81" s="27"/>
       <c r="H81" s="18"/>
-      <c r="I81" s="18"/>
-      <c r="J81" s="18"/>
-      <c r="K81" s="18"/>
-      <c r="L81" s="25"/>
-      <c r="M81" s="25"/>
-      <c r="N81" s="25"/>
+      <c r="I81" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J81" s="27"/>
+      <c r="K81" s="27"/>
+      <c r="L81" s="29"/>
+      <c r="M81" s="29"/>
+      <c r="N81" s="29"/>
     </row>
     <row r="82" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B82" s="27"/>
+      <c r="B82" s="35"/>
     </row>
     <row r="83" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B83" s="27"/>
-      <c r="D83" s="26" t="s">
+      <c r="B83" s="35"/>
+      <c r="D83" s="28" t="s">
         <v>109</v>
       </c>
       <c r="E83" s="18" t="s">
@@ -3057,119 +3182,176 @@
       <c r="F83" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G83" s="21"/>
-      <c r="H83" s="18"/>
-      <c r="I83" s="18"/>
-      <c r="J83" s="18"/>
-      <c r="K83" s="18"/>
-      <c r="L83" s="25"/>
-      <c r="M83" s="25"/>
-      <c r="N83" s="25"/>
+      <c r="G83" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="H83" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="I83" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J83" s="27">
+        <v>0.204586696749333</v>
+      </c>
+      <c r="K83" s="27">
+        <v>0.213985952346849</v>
+      </c>
+      <c r="L83" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="M83" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="N83" s="29">
+        <v>19445</v>
+      </c>
     </row>
     <row r="84" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B84" s="27"/>
-      <c r="D84" s="26"/>
+      <c r="B84" s="35"/>
+      <c r="D84" s="28"/>
       <c r="E84" s="18"/>
       <c r="F84" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G84" s="7"/>
-      <c r="H84" s="18"/>
-      <c r="I84" s="18"/>
-      <c r="J84" s="18"/>
-      <c r="K84" s="18"/>
-      <c r="L84" s="25"/>
-      <c r="M84" s="25"/>
-      <c r="N84" s="25"/>
+      <c r="G84" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="H84" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="I84" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J84" s="27">
+        <v>0.24313899999999999</v>
+      </c>
+      <c r="K84" s="27">
+        <v>0.181546683325744</v>
+      </c>
+      <c r="L84" s="29"/>
+      <c r="M84" s="29"/>
+      <c r="N84" s="29"/>
     </row>
     <row r="85" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B85" s="27"/>
-      <c r="D85" s="26"/>
+      <c r="B85" s="35"/>
+      <c r="D85" s="28"/>
       <c r="E85" s="18"/>
       <c r="F85" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G85" s="18"/>
-      <c r="H85" s="18"/>
-      <c r="I85" s="18"/>
-      <c r="J85" s="18"/>
-      <c r="K85" s="18"/>
-      <c r="L85" s="25"/>
-      <c r="M85" s="25"/>
-      <c r="N85" s="25"/>
+      <c r="G85" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="H85" s="47"/>
+      <c r="I85" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="J85" s="46"/>
+      <c r="K85" s="46"/>
+      <c r="L85" s="29"/>
+      <c r="M85" s="29"/>
+      <c r="N85" s="29"/>
     </row>
     <row r="86" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B86" s="27"/>
-      <c r="D86" s="26"/>
+      <c r="B86" s="35"/>
+      <c r="D86" s="28"/>
       <c r="E86" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F86" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G86" s="18"/>
-      <c r="H86" s="18"/>
-      <c r="I86" s="18"/>
-      <c r="J86" s="18"/>
-      <c r="K86" s="18"/>
-      <c r="L86" s="25"/>
-      <c r="M86" s="25"/>
-      <c r="N86" s="25"/>
+      <c r="G86" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="H86" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I86" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J86" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="K86" s="27">
+        <v>0.17957555142145301</v>
+      </c>
+      <c r="L86" s="29"/>
+      <c r="M86" s="29"/>
+      <c r="N86" s="29"/>
     </row>
     <row r="87" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B87" s="27"/>
-      <c r="D87" s="26"/>
+      <c r="B87" s="35"/>
+      <c r="D87" s="28"/>
       <c r="E87" s="18"/>
       <c r="F87" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G87" s="18"/>
-      <c r="H87" s="18"/>
-      <c r="I87" s="18"/>
-      <c r="J87" s="18"/>
-      <c r="K87" s="7"/>
-      <c r="L87" s="25"/>
-      <c r="M87" s="25"/>
-      <c r="N87" s="25"/>
+      <c r="G87" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H87" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I87" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J87" s="27">
+        <v>0.52178599999999997</v>
+      </c>
+      <c r="K87" s="27">
+        <v>18.97</v>
+      </c>
+      <c r="L87" s="29"/>
+      <c r="M87" s="29"/>
+      <c r="N87" s="29"/>
     </row>
     <row r="88" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B88" s="27"/>
-      <c r="D88" s="26"/>
+      <c r="B88" s="35"/>
+      <c r="D88" s="28"/>
       <c r="E88" s="18"/>
       <c r="F88" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G88" s="18"/>
-      <c r="H88" s="18"/>
-      <c r="I88" s="18"/>
-      <c r="J88" s="18"/>
-      <c r="K88" s="18"/>
-      <c r="L88" s="25"/>
-      <c r="M88" s="25"/>
-      <c r="N88" s="25"/>
+      <c r="G88" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="H88" s="47"/>
+      <c r="I88" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="J88" s="46"/>
+      <c r="K88" s="46"/>
+      <c r="L88" s="29"/>
+      <c r="M88" s="29"/>
+      <c r="N88" s="29"/>
     </row>
     <row r="89" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B89" s="27"/>
-      <c r="D89" s="26"/>
+      <c r="B89" s="35"/>
+      <c r="D89" s="28"/>
       <c r="E89" s="18"/>
       <c r="F89" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="G89" s="18"/>
+      <c r="G89" s="27"/>
       <c r="H89" s="18"/>
-      <c r="I89" s="18"/>
-      <c r="J89" s="18"/>
-      <c r="K89" s="18"/>
-      <c r="L89" s="25"/>
-      <c r="M89" s="25"/>
-      <c r="N89" s="25"/>
+      <c r="I89" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J89" s="27"/>
+      <c r="K89" s="27"/>
+      <c r="L89" s="29"/>
+      <c r="M89" s="29"/>
+      <c r="N89" s="29"/>
     </row>
     <row r="90" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B90" s="27"/>
+      <c r="B90" s="35"/>
+      <c r="G90" s="45"/>
     </row>
     <row r="91" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B91" s="27"/>
-      <c r="D91" s="26" t="s">
+      <c r="B91" s="35"/>
+      <c r="D91" s="28" t="s">
         <v>110</v>
       </c>
       <c r="E91" s="18" t="s">
@@ -3178,115 +3360,165 @@
       <c r="F91" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G91" s="21"/>
+      <c r="G91" s="26"/>
       <c r="H91" s="18"/>
-      <c r="I91" s="18"/>
-      <c r="J91" s="18"/>
-      <c r="K91" s="18"/>
-      <c r="L91" s="25"/>
-      <c r="M91" s="25"/>
-      <c r="N91" s="25"/>
+      <c r="I91" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J91" s="27"/>
+      <c r="K91" s="27"/>
+      <c r="L91" s="29"/>
+      <c r="M91" s="29"/>
+      <c r="N91" s="29"/>
     </row>
     <row r="92" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B92" s="27"/>
-      <c r="D92" s="26"/>
+      <c r="B92" s="35"/>
+      <c r="D92" s="28"/>
       <c r="E92" s="18"/>
       <c r="F92" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G92" s="7"/>
+      <c r="G92" s="27"/>
       <c r="H92" s="18"/>
-      <c r="I92" s="18"/>
-      <c r="J92" s="18"/>
-      <c r="K92" s="18"/>
-      <c r="L92" s="25"/>
-      <c r="M92" s="25"/>
-      <c r="N92" s="25"/>
+      <c r="I92" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J92" s="27"/>
+      <c r="K92" s="27"/>
+      <c r="L92" s="29"/>
+      <c r="M92" s="29"/>
+      <c r="N92" s="29"/>
     </row>
     <row r="93" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B93" s="27"/>
-      <c r="D93" s="26"/>
+      <c r="B93" s="35"/>
+      <c r="D93" s="28"/>
       <c r="E93" s="18"/>
       <c r="F93" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G93" s="18"/>
+      <c r="G93" s="27"/>
       <c r="H93" s="18"/>
-      <c r="I93" s="18"/>
-      <c r="J93" s="18"/>
-      <c r="K93" s="18"/>
-      <c r="L93" s="25"/>
-      <c r="M93" s="25"/>
-      <c r="N93" s="25"/>
+      <c r="I93" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J93" s="27"/>
+      <c r="K93" s="27"/>
+      <c r="L93" s="29"/>
+      <c r="M93" s="29"/>
+      <c r="N93" s="29"/>
     </row>
     <row r="94" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B94" s="27"/>
-      <c r="D94" s="26"/>
+      <c r="B94" s="35"/>
+      <c r="D94" s="28"/>
       <c r="E94" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F94" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G94" s="18"/>
+      <c r="G94" s="27"/>
       <c r="H94" s="18"/>
-      <c r="I94" s="18"/>
-      <c r="J94" s="18"/>
-      <c r="K94" s="18"/>
-      <c r="L94" s="25"/>
-      <c r="M94" s="25"/>
-      <c r="N94" s="25"/>
+      <c r="I94" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J94" s="27"/>
+      <c r="K94" s="27"/>
+      <c r="L94" s="29"/>
+      <c r="M94" s="29"/>
+      <c r="N94" s="29"/>
     </row>
     <row r="95" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B95" s="27"/>
-      <c r="D95" s="26"/>
+      <c r="B95" s="35"/>
+      <c r="D95" s="28"/>
       <c r="E95" s="18"/>
       <c r="F95" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G95" s="18"/>
+      <c r="G95" s="27"/>
       <c r="H95" s="18"/>
-      <c r="I95" s="18"/>
-      <c r="J95" s="18"/>
-      <c r="K95" s="7"/>
-      <c r="L95" s="25"/>
-      <c r="M95" s="25"/>
-      <c r="N95" s="25"/>
+      <c r="I95" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J95" s="27"/>
+      <c r="K95" s="27"/>
+      <c r="L95" s="29"/>
+      <c r="M95" s="29"/>
+      <c r="N95" s="29"/>
     </row>
     <row r="96" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B96" s="27"/>
-      <c r="D96" s="26"/>
+      <c r="B96" s="35"/>
+      <c r="D96" s="28"/>
       <c r="E96" s="18"/>
       <c r="F96" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G96" s="18"/>
+      <c r="G96" s="27"/>
       <c r="H96" s="18"/>
-      <c r="I96" s="18"/>
-      <c r="J96" s="18"/>
-      <c r="K96" s="18"/>
-      <c r="L96" s="25"/>
-      <c r="M96" s="25"/>
-      <c r="N96" s="25"/>
+      <c r="I96" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J96" s="27"/>
+      <c r="K96" s="27"/>
+      <c r="L96" s="29"/>
+      <c r="M96" s="29"/>
+      <c r="N96" s="29"/>
     </row>
     <row r="97" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B97" s="27"/>
-      <c r="D97" s="26"/>
+      <c r="B97" s="35"/>
+      <c r="D97" s="28"/>
       <c r="E97" s="18"/>
       <c r="F97" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="G97" s="18"/>
+      <c r="G97" s="27"/>
       <c r="H97" s="18"/>
-      <c r="I97" s="18"/>
-      <c r="J97" s="18"/>
-      <c r="K97" s="18"/>
-      <c r="L97" s="25"/>
-      <c r="M97" s="25"/>
-      <c r="N97" s="25"/>
+      <c r="I97" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J97" s="27"/>
+      <c r="K97" s="27"/>
+      <c r="L97" s="29"/>
+      <c r="M97" s="29"/>
+      <c r="N97" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="N59:N65"/>
+    <mergeCell ref="M27:M33"/>
+    <mergeCell ref="M35:M41"/>
+    <mergeCell ref="M43:M49"/>
+    <mergeCell ref="M51:M57"/>
+    <mergeCell ref="M59:M65"/>
+    <mergeCell ref="M19:M25"/>
+    <mergeCell ref="N27:N33"/>
+    <mergeCell ref="N35:N41"/>
+    <mergeCell ref="N43:N49"/>
+    <mergeCell ref="N51:N57"/>
+    <mergeCell ref="B2:B33"/>
+    <mergeCell ref="D67:D73"/>
+    <mergeCell ref="L67:L73"/>
+    <mergeCell ref="M67:M73"/>
+    <mergeCell ref="N67:N73"/>
+    <mergeCell ref="B35:B65"/>
+    <mergeCell ref="L43:L49"/>
+    <mergeCell ref="L51:L57"/>
+    <mergeCell ref="L59:L65"/>
+    <mergeCell ref="L2:L9"/>
+    <mergeCell ref="L11:L17"/>
+    <mergeCell ref="L19:L25"/>
+    <mergeCell ref="L27:L33"/>
+    <mergeCell ref="L35:L41"/>
+    <mergeCell ref="D59:D65"/>
+    <mergeCell ref="D43:D49"/>
+    <mergeCell ref="B67:B97"/>
+    <mergeCell ref="D75:D81"/>
+    <mergeCell ref="L75:L81"/>
+    <mergeCell ref="M75:M81"/>
+    <mergeCell ref="N75:N81"/>
+    <mergeCell ref="D83:D89"/>
+    <mergeCell ref="L83:L89"/>
+    <mergeCell ref="M83:M89"/>
+    <mergeCell ref="N83:N89"/>
     <mergeCell ref="R2:U2"/>
     <mergeCell ref="D91:D97"/>
     <mergeCell ref="L91:L97"/>
@@ -3303,42 +3535,6 @@
     <mergeCell ref="N19:N25"/>
     <mergeCell ref="M2:M9"/>
     <mergeCell ref="M11:M17"/>
-    <mergeCell ref="B67:B97"/>
-    <mergeCell ref="D75:D81"/>
-    <mergeCell ref="L75:L81"/>
-    <mergeCell ref="M75:M81"/>
-    <mergeCell ref="N75:N81"/>
-    <mergeCell ref="D83:D89"/>
-    <mergeCell ref="L83:L89"/>
-    <mergeCell ref="M83:M89"/>
-    <mergeCell ref="N83:N89"/>
-    <mergeCell ref="B2:B33"/>
-    <mergeCell ref="D67:D73"/>
-    <mergeCell ref="L67:L73"/>
-    <mergeCell ref="M67:M73"/>
-    <mergeCell ref="N67:N73"/>
-    <mergeCell ref="B35:B65"/>
-    <mergeCell ref="L43:L49"/>
-    <mergeCell ref="L51:L57"/>
-    <mergeCell ref="L59:L65"/>
-    <mergeCell ref="L2:L9"/>
-    <mergeCell ref="L11:L17"/>
-    <mergeCell ref="L19:L25"/>
-    <mergeCell ref="L27:L33"/>
-    <mergeCell ref="L35:L41"/>
-    <mergeCell ref="D59:D65"/>
-    <mergeCell ref="D43:D49"/>
-    <mergeCell ref="M19:M25"/>
-    <mergeCell ref="N27:N33"/>
-    <mergeCell ref="N35:N41"/>
-    <mergeCell ref="N43:N49"/>
-    <mergeCell ref="N51:N57"/>
-    <mergeCell ref="N59:N65"/>
-    <mergeCell ref="M27:M33"/>
-    <mergeCell ref="M35:M41"/>
-    <mergeCell ref="M43:M49"/>
-    <mergeCell ref="M51:M57"/>
-    <mergeCell ref="M59:M65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
update results (3 tests left)
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="138">
   <si>
     <t>Ferramenta</t>
   </si>
@@ -416,6 +416,27 @@
   </si>
   <si>
     <t>01m46.66s</t>
+  </si>
+  <si>
+    <t>Melhor: 0.7715</t>
+  </si>
+  <si>
+    <t>3m43s</t>
+  </si>
+  <si>
+    <t>25m33.801s</t>
+  </si>
+  <si>
+    <t>11m03.614s</t>
+  </si>
+  <si>
+    <t>2m21.35s</t>
+  </si>
+  <si>
+    <t>10m16.991281s</t>
+  </si>
+  <si>
+    <t>4m19s</t>
   </si>
 </sst>
 </file>
@@ -528,7 +549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -611,6 +632,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -660,15 +696,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -953,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D61" workbookViewId="0">
-      <selection activeCell="N83" sqref="L75:N89"/>
+    <sheetView tabSelected="1" topLeftCell="D73" workbookViewId="0">
+      <selection activeCell="H89" sqref="H89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,7 +992,7 @@
     <col min="4" max="4" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" style="1" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -1021,10 +1048,10 @@
       </c>
     </row>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="33" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="2"/>
@@ -1046,25 +1073,25 @@
       <c r="K2" s="2">
         <v>2.3615173893038102</v>
       </c>
-      <c r="L2" s="37" t="s">
+      <c r="L2" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="M2" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="N2" s="35">
+      <c r="N2" s="40">
         <v>73</v>
       </c>
-      <c r="R2" s="28" t="s">
+      <c r="R2" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="28"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
     </row>
     <row r="3" spans="2:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="28"/>
-      <c r="D3" s="28"/>
+      <c r="B3" s="33"/>
+      <c r="D3" s="33"/>
       <c r="E3" s="2" t="s">
         <v>20</v>
       </c>
@@ -1086,9 +1113,9 @@
       <c r="K3" s="2">
         <v>2.2556710599482699</v>
       </c>
-      <c r="L3" s="38"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
       <c r="R3" s="19" t="s">
         <v>2</v>
       </c>
@@ -1103,8 +1130,8 @@
       </c>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B4" s="28"/>
-      <c r="D4" s="28"/>
+      <c r="B4" s="33"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
         <v>15</v>
@@ -1124,9 +1151,9 @@
       <c r="K4" s="2">
         <v>2.2502649752898698</v>
       </c>
-      <c r="L4" s="38"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
       <c r="R4" s="19" t="s">
         <v>3</v>
       </c>
@@ -1141,8 +1168,8 @@
       </c>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="28"/>
-      <c r="D5" s="28"/>
+      <c r="B5" s="33"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
         <v>17</v>
@@ -1162,9 +1189,9 @@
       <c r="K5" s="7">
         <v>2.0563812623190301</v>
       </c>
-      <c r="L5" s="38"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
       <c r="R5" s="19" t="s">
         <v>28</v>
       </c>
@@ -1179,8 +1206,8 @@
       </c>
     </row>
     <row r="6" spans="2:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="28"/>
-      <c r="D6" s="28"/>
+      <c r="B6" s="33"/>
+      <c r="D6" s="33"/>
       <c r="E6" s="5" t="s">
         <v>36</v>
       </c>
@@ -1202,9 +1229,9 @@
       <c r="K6" s="4">
         <v>2.5263518439219701</v>
       </c>
-      <c r="L6" s="38"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
       <c r="R6" s="19" t="s">
         <v>38</v>
       </c>
@@ -1219,8 +1246,8 @@
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="28"/>
-      <c r="D7" s="28"/>
+      <c r="B7" s="33"/>
+      <c r="D7" s="33"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
         <v>23</v>
@@ -1240,9 +1267,9 @@
       <c r="K7" s="2">
         <v>2.29</v>
       </c>
-      <c r="L7" s="38"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="35"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
       <c r="R7" s="19" t="s">
         <v>44</v>
       </c>
@@ -1257,8 +1284,8 @@
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="28"/>
-      <c r="D8" s="28"/>
+      <c r="B8" s="33"/>
+      <c r="D8" s="33"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
         <v>25</v>
@@ -1278,9 +1305,9 @@
       <c r="K8" s="4">
         <v>2.0925560658435201</v>
       </c>
-      <c r="L8" s="38"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="35"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="40"/>
       <c r="R8" s="19" t="s">
         <v>50</v>
       </c>
@@ -1295,8 +1322,8 @@
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="28"/>
-      <c r="D9" s="31"/>
+      <c r="B9" s="33"/>
+      <c r="D9" s="36"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8" t="s">
         <v>26</v>
@@ -1308,9 +1335,9 @@
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="35"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
       <c r="R9" s="19" t="s">
         <v>57</v>
       </c>
@@ -1325,7 +1352,7 @@
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="28"/>
+      <c r="B10" s="33"/>
       <c r="D10" s="12"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
@@ -1351,8 +1378,8 @@
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="28"/>
-      <c r="D11" s="32" t="s">
+      <c r="B11" s="33"/>
+      <c r="D11" s="37" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="9" t="s">
@@ -1376,13 +1403,13 @@
       <c r="K11" s="16">
         <v>42.172544929804403</v>
       </c>
-      <c r="L11" s="40" t="s">
+      <c r="L11" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="M11" s="36" t="s">
+      <c r="M11" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="N11" s="36">
+      <c r="N11" s="41">
         <v>160</v>
       </c>
       <c r="R11" s="19" t="s">
@@ -1399,8 +1426,8 @@
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="28"/>
-      <c r="D12" s="33"/>
+      <c r="B12" s="33"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
         <v>15</v>
@@ -1420,9 +1447,9 @@
       <c r="K12" s="4">
         <v>42.4696075892439</v>
       </c>
-      <c r="L12" s="41"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
       <c r="R12" s="19" t="s">
         <v>103</v>
       </c>
@@ -1437,8 +1464,8 @@
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="28"/>
-      <c r="D13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="D13" s="38"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
         <v>17</v>
@@ -1458,9 +1485,9 @@
       <c r="K13" s="4">
         <v>43.043253511127602</v>
       </c>
-      <c r="L13" s="41"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="36"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
       <c r="R13" s="20" t="s">
         <v>108</v>
       </c>
@@ -1475,8 +1502,8 @@
       </c>
     </row>
     <row r="14" spans="2:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="28"/>
-      <c r="D14" s="33"/>
+      <c r="B14" s="33"/>
+      <c r="D14" s="38"/>
       <c r="E14" s="5" t="s">
         <v>36</v>
       </c>
@@ -1498,9 +1525,9 @@
       <c r="K14" s="4">
         <v>42.455950916767499</v>
       </c>
-      <c r="L14" s="41"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
       <c r="R14" s="20" t="s">
         <v>109</v>
       </c>
@@ -1515,8 +1542,8 @@
       </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B15" s="28"/>
-      <c r="D15" s="33"/>
+      <c r="B15" s="33"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4" t="s">
         <v>23</v>
@@ -1536,9 +1563,9 @@
       <c r="K15" s="4">
         <v>42.61</v>
       </c>
-      <c r="L15" s="41"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="36"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41"/>
       <c r="R15" s="20" t="s">
         <v>110</v>
       </c>
@@ -1553,8 +1580,8 @@
       </c>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B16" s="28"/>
-      <c r="D16" s="33"/>
+      <c r="B16" s="33"/>
+      <c r="D16" s="38"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
         <v>25</v>
@@ -1574,13 +1601,13 @@
       <c r="K16" s="4">
         <v>42.954693127434403</v>
       </c>
-      <c r="L16" s="41"/>
-      <c r="M16" s="36"/>
-      <c r="N16" s="36"/>
+      <c r="L16" s="46"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="41"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="28"/>
-      <c r="D17" s="34"/>
+      <c r="B17" s="33"/>
+      <c r="D17" s="39"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8" t="s">
         <v>26</v>
@@ -1592,12 +1619,12 @@
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="36"/>
-      <c r="N17" s="36"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="41"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="28"/>
+      <c r="B18" s="33"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
@@ -1611,8 +1638,8 @@
       <c r="N18" s="11"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="28"/>
-      <c r="D19" s="32" t="s">
+      <c r="B19" s="33"/>
+      <c r="D19" s="37" t="s">
         <v>38</v>
       </c>
       <c r="E19" s="9" t="s">
@@ -1636,19 +1663,19 @@
       <c r="K19" s="9">
         <v>0.23469975874427401</v>
       </c>
-      <c r="L19" s="43" t="s">
+      <c r="L19" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="M19" s="29" t="s">
+      <c r="M19" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="N19" s="29">
+      <c r="N19" s="34">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="28"/>
-      <c r="D20" s="33"/>
+      <c r="B20" s="33"/>
+      <c r="D20" s="38"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
         <v>15</v>
@@ -1668,13 +1695,13 @@
       <c r="K20" s="4">
         <v>0.26615681314328199</v>
       </c>
-      <c r="L20" s="44"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="29"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="28"/>
-      <c r="D21" s="33"/>
+      <c r="B21" s="33"/>
+      <c r="D21" s="38"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
         <v>17</v>
@@ -1694,13 +1721,13 @@
       <c r="K21" s="4">
         <v>0.27054514227366</v>
       </c>
-      <c r="L21" s="44"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="29"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
     </row>
     <row r="22" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="28"/>
-      <c r="D22" s="33"/>
+      <c r="B22" s="33"/>
+      <c r="D22" s="38"/>
       <c r="E22" s="5" t="s">
         <v>36</v>
       </c>
@@ -1722,13 +1749,13 @@
       <c r="K22" s="7">
         <v>0.23440350034482499</v>
       </c>
-      <c r="L22" s="44"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="29"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="28"/>
-      <c r="D23" s="33"/>
+      <c r="B23" s="33"/>
+      <c r="D23" s="38"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4" t="s">
         <v>23</v>
@@ -1748,13 +1775,13 @@
       <c r="K23" s="4">
         <v>0.27</v>
       </c>
-      <c r="L23" s="44"/>
-      <c r="M23" s="29"/>
-      <c r="N23" s="29"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="34"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="28"/>
-      <c r="D24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="D24" s="38"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4" t="s">
         <v>25</v>
@@ -1774,13 +1801,13 @@
       <c r="K24" s="4">
         <v>0.24189871737548899</v>
       </c>
-      <c r="L24" s="44"/>
-      <c r="M24" s="29"/>
-      <c r="N24" s="29"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="28"/>
-      <c r="D25" s="34"/>
+      <c r="B25" s="33"/>
+      <c r="D25" s="39"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8" t="s">
         <v>26</v>
@@ -1792,12 +1819,12 @@
       </c>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="29"/>
-      <c r="N25" s="29"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="34"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="28"/>
+      <c r="B26" s="33"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
@@ -1811,8 +1838,8 @@
       <c r="N26" s="11"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="28"/>
-      <c r="D27" s="32" t="s">
+      <c r="B27" s="33"/>
+      <c r="D27" s="37" t="s">
         <v>45</v>
       </c>
       <c r="E27" s="9" t="s">
@@ -1836,19 +1863,19 @@
       <c r="K27" s="9">
         <v>141.96334027640401</v>
       </c>
-      <c r="L27" s="43" t="s">
+      <c r="L27" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="M27" s="29" t="s">
+      <c r="M27" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="N27" s="29">
+      <c r="N27" s="34">
         <v>15</v>
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="28"/>
-      <c r="D28" s="33"/>
+      <c r="B28" s="33"/>
+      <c r="D28" s="38"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4" t="s">
         <v>15</v>
@@ -1868,13 +1895,13 @@
       <c r="K28" s="4">
         <v>146.72373452591</v>
       </c>
-      <c r="L28" s="44"/>
-      <c r="M28" s="29"/>
-      <c r="N28" s="29"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="34"/>
+      <c r="N28" s="34"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="28"/>
-      <c r="D29" s="33"/>
+      <c r="B29" s="33"/>
+      <c r="D29" s="38"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4" t="s">
         <v>17</v>
@@ -1894,13 +1921,13 @@
       <c r="K29" s="7">
         <v>140.69022615456799</v>
       </c>
-      <c r="L29" s="44"/>
-      <c r="M29" s="29"/>
-      <c r="N29" s="29"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="34"/>
+      <c r="N29" s="34"/>
     </row>
     <row r="30" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B30" s="28"/>
-      <c r="D30" s="33"/>
+      <c r="B30" s="33"/>
+      <c r="D30" s="38"/>
       <c r="E30" s="5" t="s">
         <v>36</v>
       </c>
@@ -1922,13 +1949,13 @@
       <c r="K30" s="4">
         <v>142.52852874723999</v>
       </c>
-      <c r="L30" s="44"/>
-      <c r="M30" s="29"/>
-      <c r="N30" s="29"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="34"/>
+      <c r="N30" s="34"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="28"/>
-      <c r="D31" s="33"/>
+      <c r="B31" s="33"/>
+      <c r="D31" s="38"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4" t="s">
         <v>23</v>
@@ -1948,13 +1975,13 @@
       <c r="K31" s="4">
         <v>152.29</v>
       </c>
-      <c r="L31" s="44"/>
-      <c r="M31" s="29"/>
-      <c r="N31" s="29"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="34"/>
+      <c r="N31" s="34"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B32" s="28"/>
-      <c r="D32" s="33"/>
+      <c r="B32" s="33"/>
+      <c r="D32" s="38"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4" t="s">
         <v>25</v>
@@ -1974,13 +2001,13 @@
       <c r="K32" s="4">
         <v>144.833568734441</v>
       </c>
-      <c r="L32" s="44"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
+      <c r="L32" s="49"/>
+      <c r="M32" s="34"/>
+      <c r="N32" s="34"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="28"/>
-      <c r="D33" s="34"/>
+      <c r="B33" s="33"/>
+      <c r="D33" s="39"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8" t="s">
         <v>26</v>
@@ -1992,9 +2019,9 @@
       </c>
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
-      <c r="L33" s="32"/>
-      <c r="M33" s="29"/>
-      <c r="N33" s="29"/>
+      <c r="L33" s="37"/>
+      <c r="M33" s="34"/>
+      <c r="N33" s="34"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D34" s="13"/>
@@ -2010,10 +2037,10 @@
       <c r="N34" s="11"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="35" t="s">
+      <c r="B35" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="30" t="s">
+      <c r="D35" s="35" t="s">
         <v>50</v>
       </c>
       <c r="E35" s="9" t="s">
@@ -2037,19 +2064,19 @@
       <c r="K35" s="9">
         <v>0.910468209203948</v>
       </c>
-      <c r="L35" s="43" t="s">
+      <c r="L35" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="M35" s="29" t="s">
+      <c r="M35" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="N35" s="29">
+      <c r="N35" s="34">
         <v>5132</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B36" s="35"/>
-      <c r="D36" s="28"/>
+      <c r="B36" s="40"/>
+      <c r="D36" s="33"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4" t="s">
         <v>15</v>
@@ -2069,13 +2096,13 @@
       <c r="K36" s="4">
         <v>0.88615775755244997</v>
       </c>
-      <c r="L36" s="44"/>
-      <c r="M36" s="29"/>
-      <c r="N36" s="29"/>
+      <c r="L36" s="49"/>
+      <c r="M36" s="34"/>
+      <c r="N36" s="34"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="35"/>
-      <c r="D37" s="28"/>
+      <c r="B37" s="40"/>
+      <c r="D37" s="33"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4" t="s">
         <v>17</v>
@@ -2095,13 +2122,13 @@
       <c r="K37" s="4">
         <v>0.87077511430158505</v>
       </c>
-      <c r="L37" s="44"/>
-      <c r="M37" s="29"/>
-      <c r="N37" s="29"/>
+      <c r="L37" s="49"/>
+      <c r="M37" s="34"/>
+      <c r="N37" s="34"/>
     </row>
     <row r="38" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B38" s="35"/>
-      <c r="D38" s="28"/>
+      <c r="B38" s="40"/>
+      <c r="D38" s="33"/>
       <c r="E38" s="5" t="s">
         <v>36</v>
       </c>
@@ -2123,13 +2150,13 @@
       <c r="K38" s="4">
         <v>0.91063111566893096</v>
       </c>
-      <c r="L38" s="44"/>
-      <c r="M38" s="29"/>
-      <c r="N38" s="29"/>
+      <c r="L38" s="49"/>
+      <c r="M38" s="34"/>
+      <c r="N38" s="34"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B39" s="35"/>
-      <c r="D39" s="28"/>
+      <c r="B39" s="40"/>
+      <c r="D39" s="33"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4" t="s">
         <v>23</v>
@@ -2149,13 +2176,13 @@
       <c r="K39" s="4">
         <v>0.91</v>
       </c>
-      <c r="L39" s="44"/>
-      <c r="M39" s="29"/>
-      <c r="N39" s="29"/>
+      <c r="L39" s="49"/>
+      <c r="M39" s="34"/>
+      <c r="N39" s="34"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B40" s="35"/>
-      <c r="D40" s="28"/>
+      <c r="B40" s="40"/>
+      <c r="D40" s="33"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4" t="s">
         <v>25</v>
@@ -2175,13 +2202,13 @@
       <c r="K40" s="7">
         <v>0.91188896722642299</v>
       </c>
-      <c r="L40" s="44"/>
-      <c r="M40" s="29"/>
-      <c r="N40" s="29"/>
+      <c r="L40" s="49"/>
+      <c r="M40" s="34"/>
+      <c r="N40" s="34"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B41" s="35"/>
-      <c r="D41" s="31"/>
+      <c r="B41" s="40"/>
+      <c r="D41" s="36"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8" t="s">
         <v>26</v>
@@ -2193,12 +2220,12 @@
       </c>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
-      <c r="L41" s="32"/>
-      <c r="M41" s="29"/>
-      <c r="N41" s="29"/>
+      <c r="L41" s="37"/>
+      <c r="M41" s="34"/>
+      <c r="N41" s="34"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B42" s="35"/>
+      <c r="B42" s="40"/>
       <c r="D42" s="12"/>
       <c r="E42" s="13"/>
       <c r="F42" s="13"/>
@@ -2212,8 +2239,8 @@
       <c r="N42" s="11"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B43" s="35"/>
-      <c r="D43" s="30" t="s">
+      <c r="B43" s="40"/>
+      <c r="D43" s="35" t="s">
         <v>57</v>
       </c>
       <c r="E43" s="9" t="s">
@@ -2237,19 +2264,19 @@
       <c r="K43" s="9">
         <v>0.78503433208489304</v>
       </c>
-      <c r="L43" s="29" t="s">
+      <c r="L43" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="M43" s="29" t="s">
+      <c r="M43" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="N43" s="29">
+      <c r="N43" s="34">
         <v>419021</v>
       </c>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B44" s="35"/>
-      <c r="D44" s="28"/>
+      <c r="B44" s="40"/>
+      <c r="D44" s="33"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4" t="s">
         <v>15</v>
@@ -2269,13 +2296,13 @@
       <c r="K44" s="4">
         <v>0.59706616729088602</v>
       </c>
-      <c r="L44" s="33"/>
-      <c r="M44" s="29"/>
-      <c r="N44" s="29"/>
+      <c r="L44" s="38"/>
+      <c r="M44" s="34"/>
+      <c r="N44" s="34"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B45" s="35"/>
-      <c r="D45" s="28"/>
+      <c r="B45" s="40"/>
+      <c r="D45" s="33"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4" t="s">
         <v>17</v>
@@ -2295,13 +2322,13 @@
       <c r="K45" s="4">
         <v>0.71168851435705305</v>
       </c>
-      <c r="L45" s="33"/>
-      <c r="M45" s="29"/>
-      <c r="N45" s="29"/>
+      <c r="L45" s="38"/>
+      <c r="M45" s="34"/>
+      <c r="N45" s="34"/>
     </row>
     <row r="46" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B46" s="35"/>
-      <c r="D46" s="28"/>
+      <c r="B46" s="40"/>
+      <c r="D46" s="33"/>
       <c r="E46" s="5" t="s">
         <v>36</v>
       </c>
@@ -2323,13 +2350,13 @@
       <c r="K46" s="4">
         <v>0.77699750312109805</v>
       </c>
-      <c r="L46" s="33"/>
-      <c r="M46" s="29"/>
-      <c r="N46" s="29"/>
+      <c r="L46" s="38"/>
+      <c r="M46" s="34"/>
+      <c r="N46" s="34"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B47" s="35"/>
-      <c r="D47" s="28"/>
+      <c r="B47" s="40"/>
+      <c r="D47" s="33"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4" t="s">
         <v>23</v>
@@ -2349,13 +2376,13 @@
       <c r="K47" s="7">
         <v>0.8</v>
       </c>
-      <c r="L47" s="33"/>
-      <c r="M47" s="29"/>
-      <c r="N47" s="29"/>
+      <c r="L47" s="38"/>
+      <c r="M47" s="34"/>
+      <c r="N47" s="34"/>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B48" s="35"/>
-      <c r="D48" s="28"/>
+      <c r="B48" s="40"/>
+      <c r="D48" s="33"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4" t="s">
         <v>25</v>
@@ -2375,13 +2402,13 @@
       <c r="K48" s="7">
         <v>0.80024968789013695</v>
       </c>
-      <c r="L48" s="33"/>
-      <c r="M48" s="29"/>
-      <c r="N48" s="29"/>
+      <c r="L48" s="38"/>
+      <c r="M48" s="34"/>
+      <c r="N48" s="34"/>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B49" s="35"/>
-      <c r="D49" s="31"/>
+      <c r="B49" s="40"/>
+      <c r="D49" s="36"/>
       <c r="E49" s="8"/>
       <c r="F49" s="8" t="s">
         <v>26</v>
@@ -2393,12 +2420,12 @@
       </c>
       <c r="J49" s="8"/>
       <c r="K49" s="8"/>
-      <c r="L49" s="33"/>
-      <c r="M49" s="29"/>
-      <c r="N49" s="29"/>
+      <c r="L49" s="38"/>
+      <c r="M49" s="34"/>
+      <c r="N49" s="34"/>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B50" s="35"/>
+      <c r="B50" s="40"/>
       <c r="D50" s="12"/>
       <c r="E50" s="13"/>
       <c r="F50" s="13"/>
@@ -2412,8 +2439,8 @@
       <c r="N50" s="11"/>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B51" s="35"/>
-      <c r="D51" s="30" t="s">
+      <c r="B51" s="40"/>
+      <c r="D51" s="35" t="s">
         <v>62</v>
       </c>
       <c r="E51" s="9" t="s">
@@ -2437,19 +2464,19 @@
       <c r="K51" s="9">
         <v>0.94655497110201903</v>
       </c>
-      <c r="L51" s="29" t="s">
+      <c r="L51" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="M51" s="29" t="s">
+      <c r="M51" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="N51" s="29">
+      <c r="N51" s="34">
         <v>147659</v>
       </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B52" s="35"/>
-      <c r="D52" s="28"/>
+      <c r="B52" s="40"/>
+      <c r="D52" s="33"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4" t="s">
         <v>15</v>
@@ -2469,13 +2496,13 @@
       <c r="K52" s="4">
         <v>0.83995714007403</v>
       </c>
-      <c r="L52" s="33"/>
-      <c r="M52" s="29"/>
-      <c r="N52" s="29"/>
+      <c r="L52" s="38"/>
+      <c r="M52" s="34"/>
+      <c r="N52" s="34"/>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B53" s="35"/>
-      <c r="D53" s="28"/>
+      <c r="B53" s="40"/>
+      <c r="D53" s="33"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4" t="s">
         <v>17</v>
@@ -2495,13 +2522,13 @@
       <c r="K53" s="7">
         <v>1</v>
       </c>
-      <c r="L53" s="33"/>
-      <c r="M53" s="29"/>
-      <c r="N53" s="29"/>
+      <c r="L53" s="38"/>
+      <c r="M53" s="34"/>
+      <c r="N53" s="34"/>
     </row>
     <row r="54" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B54" s="35"/>
-      <c r="D54" s="28"/>
+      <c r="B54" s="40"/>
+      <c r="D54" s="33"/>
       <c r="E54" s="5" t="s">
         <v>36</v>
       </c>
@@ -2523,13 +2550,13 @@
       <c r="K54" s="4">
         <v>0.97873848082154702</v>
       </c>
-      <c r="L54" s="33"/>
-      <c r="M54" s="29"/>
-      <c r="N54" s="29"/>
+      <c r="L54" s="38"/>
+      <c r="M54" s="34"/>
+      <c r="N54" s="34"/>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B55" s="35"/>
-      <c r="D55" s="28"/>
+      <c r="B55" s="40"/>
+      <c r="D55" s="33"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4" t="s">
         <v>23</v>
@@ -2549,13 +2576,13 @@
       <c r="K55" s="4">
         <v>0.94</v>
       </c>
-      <c r="L55" s="33"/>
-      <c r="M55" s="29"/>
-      <c r="N55" s="29"/>
+      <c r="L55" s="38"/>
+      <c r="M55" s="34"/>
+      <c r="N55" s="34"/>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B56" s="35"/>
-      <c r="D56" s="28"/>
+      <c r="B56" s="40"/>
+      <c r="D56" s="33"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4" t="s">
         <v>25</v>
@@ -2575,13 +2602,13 @@
       <c r="K56" s="7">
         <v>1</v>
       </c>
-      <c r="L56" s="33"/>
-      <c r="M56" s="29"/>
-      <c r="N56" s="29"/>
+      <c r="L56" s="38"/>
+      <c r="M56" s="34"/>
+      <c r="N56" s="34"/>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B57" s="35"/>
-      <c r="D57" s="31"/>
+      <c r="B57" s="40"/>
+      <c r="D57" s="36"/>
       <c r="E57" s="8"/>
       <c r="F57" s="8" t="s">
         <v>26</v>
@@ -2593,12 +2620,12 @@
       </c>
       <c r="J57" s="8"/>
       <c r="K57" s="8"/>
-      <c r="L57" s="33"/>
-      <c r="M57" s="29"/>
-      <c r="N57" s="29"/>
+      <c r="L57" s="38"/>
+      <c r="M57" s="34"/>
+      <c r="N57" s="34"/>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B58" s="35"/>
+      <c r="B58" s="40"/>
       <c r="D58" s="12"/>
       <c r="E58" s="13"/>
       <c r="F58" s="13"/>
@@ -2612,8 +2639,8 @@
       <c r="N58" s="11"/>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B59" s="35"/>
-      <c r="D59" s="28" t="s">
+      <c r="B59" s="40"/>
+      <c r="D59" s="33" t="s">
         <v>103</v>
       </c>
       <c r="E59" s="18" t="s">
@@ -2637,19 +2664,19 @@
       <c r="K59" s="27">
         <v>0.80959113938965399</v>
       </c>
-      <c r="L59" s="29" t="s">
+      <c r="L59" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="M59" s="29" t="s">
+      <c r="M59" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="N59" s="29">
+      <c r="N59" s="34">
         <v>132164</v>
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B60" s="35"/>
-      <c r="D60" s="28"/>
+      <c r="B60" s="40"/>
+      <c r="D60" s="33"/>
       <c r="E60" s="18"/>
       <c r="F60" s="18" t="s">
         <v>15</v>
@@ -2669,13 +2696,13 @@
       <c r="K60" s="27">
         <v>0.72940968540120099</v>
       </c>
-      <c r="L60" s="29"/>
-      <c r="M60" s="29"/>
-      <c r="N60" s="29"/>
+      <c r="L60" s="34"/>
+      <c r="M60" s="34"/>
+      <c r="N60" s="34"/>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B61" s="35"/>
-      <c r="D61" s="28"/>
+      <c r="B61" s="40"/>
+      <c r="D61" s="33"/>
       <c r="E61" s="18"/>
       <c r="F61" s="18" t="s">
         <v>17</v>
@@ -2695,13 +2722,13 @@
       <c r="K61" s="27">
         <v>0.65676917638741605</v>
       </c>
-      <c r="L61" s="29"/>
-      <c r="M61" s="29"/>
-      <c r="N61" s="29"/>
+      <c r="L61" s="34"/>
+      <c r="M61" s="34"/>
+      <c r="N61" s="34"/>
     </row>
     <row r="62" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B62" s="35"/>
-      <c r="D62" s="28"/>
+      <c r="B62" s="40"/>
+      <c r="D62" s="33"/>
       <c r="E62" s="17" t="s">
         <v>36</v>
       </c>
@@ -2723,13 +2750,13 @@
       <c r="K62" s="27">
         <v>0.81654294803817595</v>
       </c>
-      <c r="L62" s="29"/>
-      <c r="M62" s="29"/>
-      <c r="N62" s="29"/>
+      <c r="L62" s="34"/>
+      <c r="M62" s="34"/>
+      <c r="N62" s="34"/>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B63" s="35"/>
-      <c r="D63" s="28"/>
+      <c r="B63" s="40"/>
+      <c r="D63" s="33"/>
       <c r="E63" s="18"/>
       <c r="F63" s="18" t="s">
         <v>23</v>
@@ -2749,13 +2776,13 @@
       <c r="K63" s="27">
         <v>0.81</v>
       </c>
-      <c r="L63" s="29"/>
-      <c r="M63" s="29"/>
-      <c r="N63" s="29"/>
+      <c r="L63" s="34"/>
+      <c r="M63" s="34"/>
+      <c r="N63" s="34"/>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B64" s="35"/>
-      <c r="D64" s="28"/>
+      <c r="B64" s="40"/>
+      <c r="D64" s="33"/>
       <c r="E64" s="18"/>
       <c r="F64" s="18" t="s">
         <v>25</v>
@@ -2775,13 +2802,13 @@
       <c r="K64" s="27">
         <v>0.80452456698480002</v>
       </c>
-      <c r="L64" s="29"/>
-      <c r="M64" s="29"/>
-      <c r="N64" s="29"/>
+      <c r="L64" s="34"/>
+      <c r="M64" s="34"/>
+      <c r="N64" s="34"/>
     </row>
     <row r="65" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B65" s="35"/>
-      <c r="D65" s="28"/>
+      <c r="B65" s="40"/>
+      <c r="D65" s="33"/>
       <c r="E65" s="18"/>
       <c r="F65" s="18" t="s">
         <v>26</v>
@@ -2793,15 +2820,15 @@
       </c>
       <c r="J65" s="27"/>
       <c r="K65" s="27"/>
-      <c r="L65" s="29"/>
-      <c r="M65" s="29"/>
-      <c r="N65" s="29"/>
+      <c r="L65" s="34"/>
+      <c r="M65" s="34"/>
+      <c r="N65" s="34"/>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B67" s="35" t="s">
+      <c r="B67" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D67" s="28" t="s">
+      <c r="D67" s="33" t="s">
         <v>69</v>
       </c>
       <c r="E67" s="18" t="s">
@@ -2825,19 +2852,19 @@
       <c r="K67" s="18">
         <v>0.81557623894257503</v>
       </c>
-      <c r="L67" s="29" t="s">
+      <c r="L67" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="M67" s="29" t="s">
+      <c r="M67" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="N67" s="29">
+      <c r="N67" s="34">
         <v>23532</v>
       </c>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B68" s="35"/>
-      <c r="D68" s="28"/>
+      <c r="B68" s="40"/>
+      <c r="D68" s="33"/>
       <c r="E68" s="18"/>
       <c r="F68" s="18" t="s">
         <v>15</v>
@@ -2857,13 +2884,13 @@
       <c r="K68" s="18">
         <v>0.88222010940682705</v>
       </c>
-      <c r="L68" s="29"/>
-      <c r="M68" s="29"/>
-      <c r="N68" s="29"/>
+      <c r="L68" s="34"/>
+      <c r="M68" s="34"/>
+      <c r="N68" s="34"/>
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B69" s="35"/>
-      <c r="D69" s="28"/>
+      <c r="B69" s="40"/>
+      <c r="D69" s="33"/>
       <c r="E69" s="18"/>
       <c r="F69" s="18" t="s">
         <v>17</v>
@@ -2883,13 +2910,13 @@
       <c r="K69" s="18">
         <v>0.84568164621720798</v>
       </c>
-      <c r="L69" s="29"/>
-      <c r="M69" s="29"/>
-      <c r="N69" s="29"/>
+      <c r="L69" s="34"/>
+      <c r="M69" s="34"/>
+      <c r="N69" s="34"/>
     </row>
     <row r="70" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B70" s="35"/>
-      <c r="D70" s="28"/>
+      <c r="B70" s="40"/>
+      <c r="D70" s="33"/>
       <c r="E70" s="17" t="s">
         <v>36</v>
       </c>
@@ -2911,13 +2938,13 @@
       <c r="K70" s="18">
         <v>0.80867398669225798</v>
       </c>
-      <c r="L70" s="29"/>
-      <c r="M70" s="29"/>
-      <c r="N70" s="29"/>
+      <c r="L70" s="34"/>
+      <c r="M70" s="34"/>
+      <c r="N70" s="34"/>
     </row>
     <row r="71" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B71" s="35"/>
-      <c r="D71" s="28"/>
+      <c r="B71" s="40"/>
+      <c r="D71" s="33"/>
       <c r="E71" s="18"/>
       <c r="F71" s="18" t="s">
         <v>23</v>
@@ -2937,13 +2964,13 @@
       <c r="K71" s="7">
         <v>1</v>
       </c>
-      <c r="L71" s="29"/>
-      <c r="M71" s="29"/>
-      <c r="N71" s="29"/>
+      <c r="L71" s="34"/>
+      <c r="M71" s="34"/>
+      <c r="N71" s="34"/>
     </row>
     <row r="72" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B72" s="35"/>
-      <c r="D72" s="28"/>
+      <c r="B72" s="40"/>
+      <c r="D72" s="33"/>
       <c r="E72" s="18"/>
       <c r="F72" s="18" t="s">
         <v>25</v>
@@ -2963,13 +2990,13 @@
       <c r="K72" s="18">
         <v>0.75754008756888402</v>
       </c>
-      <c r="L72" s="29"/>
-      <c r="M72" s="29"/>
-      <c r="N72" s="29"/>
+      <c r="L72" s="34"/>
+      <c r="M72" s="34"/>
+      <c r="N72" s="34"/>
     </row>
     <row r="73" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B73" s="35"/>
-      <c r="D73" s="28"/>
+      <c r="B73" s="40"/>
+      <c r="D73" s="33"/>
       <c r="E73" s="18"/>
       <c r="F73" s="18" t="s">
         <v>26</v>
@@ -2981,16 +3008,16 @@
       </c>
       <c r="J73" s="18"/>
       <c r="K73" s="18"/>
-      <c r="L73" s="29"/>
-      <c r="M73" s="29"/>
-      <c r="N73" s="29"/>
+      <c r="L73" s="34"/>
+      <c r="M73" s="34"/>
+      <c r="N73" s="34"/>
     </row>
     <row r="74" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B74" s="35"/>
+      <c r="B74" s="40"/>
     </row>
     <row r="75" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B75" s="35"/>
-      <c r="D75" s="28" t="s">
+      <c r="B75" s="40"/>
+      <c r="D75" s="33" t="s">
         <v>108</v>
       </c>
       <c r="E75" s="18" t="s">
@@ -3014,19 +3041,19 @@
       <c r="K75" s="27">
         <v>0.55025061075102</v>
       </c>
-      <c r="L75" s="29" t="s">
+      <c r="L75" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="M75" s="29" t="s">
+      <c r="M75" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="N75" s="29">
+      <c r="N75" s="34">
         <v>21446</v>
       </c>
     </row>
     <row r="76" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B76" s="35"/>
-      <c r="D76" s="28"/>
+      <c r="B76" s="40"/>
+      <c r="D76" s="33"/>
       <c r="E76" s="18"/>
       <c r="F76" s="18" t="s">
         <v>15</v>
@@ -3046,33 +3073,33 @@
       <c r="K76" s="27">
         <v>0.55299548558353595</v>
       </c>
-      <c r="L76" s="29"/>
-      <c r="M76" s="29"/>
-      <c r="N76" s="29"/>
+      <c r="L76" s="34"/>
+      <c r="M76" s="34"/>
+      <c r="N76" s="34"/>
     </row>
     <row r="77" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B77" s="35"/>
-      <c r="D77" s="28"/>
+      <c r="B77" s="40"/>
+      <c r="D77" s="33"/>
       <c r="E77" s="18"/>
       <c r="F77" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G77" s="46" t="s">
+      <c r="G77" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="H77" s="47"/>
-      <c r="I77" s="47" t="s">
+      <c r="H77" s="31"/>
+      <c r="I77" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="J77" s="46"/>
-      <c r="K77" s="46"/>
-      <c r="L77" s="29"/>
-      <c r="M77" s="29"/>
-      <c r="N77" s="29"/>
+      <c r="J77" s="30"/>
+      <c r="K77" s="30"/>
+      <c r="L77" s="34"/>
+      <c r="M77" s="34"/>
+      <c r="N77" s="34"/>
     </row>
     <row r="78" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B78" s="35"/>
-      <c r="D78" s="28"/>
+      <c r="B78" s="40"/>
+      <c r="D78" s="33"/>
       <c r="E78" s="17" t="s">
         <v>36</v>
       </c>
@@ -3094,13 +3121,13 @@
       <c r="K78" s="27">
         <v>0.52849268592134702</v>
       </c>
-      <c r="L78" s="29"/>
-      <c r="M78" s="29"/>
-      <c r="N78" s="29"/>
+      <c r="L78" s="34"/>
+      <c r="M78" s="34"/>
+      <c r="N78" s="34"/>
     </row>
     <row r="79" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B79" s="35"/>
-      <c r="D79" s="28"/>
+      <c r="B79" s="40"/>
+      <c r="D79" s="33"/>
       <c r="E79" s="18"/>
       <c r="F79" s="18" t="s">
         <v>23</v>
@@ -3120,13 +3147,13 @@
       <c r="K79" s="27">
         <v>0.49690000000000001</v>
       </c>
-      <c r="L79" s="29"/>
-      <c r="M79" s="29"/>
-      <c r="N79" s="29"/>
+      <c r="L79" s="34"/>
+      <c r="M79" s="34"/>
+      <c r="N79" s="34"/>
     </row>
     <row r="80" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B80" s="35"/>
-      <c r="D80" s="28"/>
+      <c r="B80" s="40"/>
+      <c r="D80" s="33"/>
       <c r="E80" s="18"/>
       <c r="F80" s="18" t="s">
         <v>25</v>
@@ -3146,13 +3173,13 @@
       <c r="K80" s="27">
         <v>0.56739713139489401</v>
       </c>
-      <c r="L80" s="29"/>
-      <c r="M80" s="29"/>
-      <c r="N80" s="29"/>
+      <c r="L80" s="34"/>
+      <c r="M80" s="34"/>
+      <c r="N80" s="34"/>
     </row>
     <row r="81" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B81" s="35"/>
-      <c r="D81" s="28"/>
+      <c r="B81" s="40"/>
+      <c r="D81" s="33"/>
       <c r="E81" s="18"/>
       <c r="F81" s="18" t="s">
         <v>26</v>
@@ -3164,16 +3191,16 @@
       </c>
       <c r="J81" s="27"/>
       <c r="K81" s="27"/>
-      <c r="L81" s="29"/>
-      <c r="M81" s="29"/>
-      <c r="N81" s="29"/>
+      <c r="L81" s="34"/>
+      <c r="M81" s="34"/>
+      <c r="N81" s="34"/>
     </row>
     <row r="82" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B82" s="35"/>
+      <c r="B82" s="40"/>
     </row>
     <row r="83" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B83" s="35"/>
-      <c r="D83" s="28" t="s">
+      <c r="B83" s="40"/>
+      <c r="D83" s="33" t="s">
         <v>109</v>
       </c>
       <c r="E83" s="18" t="s">
@@ -3197,24 +3224,24 @@
       <c r="K83" s="27">
         <v>0.213985952346849</v>
       </c>
-      <c r="L83" s="29" t="s">
+      <c r="L83" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="M83" s="29" t="s">
+      <c r="M83" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="N83" s="29">
+      <c r="N83" s="34">
         <v>19445</v>
       </c>
     </row>
     <row r="84" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B84" s="35"/>
-      <c r="D84" s="28"/>
+      <c r="B84" s="40"/>
+      <c r="D84" s="33"/>
       <c r="E84" s="18"/>
       <c r="F84" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G84" s="27" t="s">
+      <c r="G84" s="7" t="s">
         <v>127</v>
       </c>
       <c r="H84" s="25" t="s">
@@ -3229,33 +3256,33 @@
       <c r="K84" s="27">
         <v>0.181546683325744</v>
       </c>
-      <c r="L84" s="29"/>
-      <c r="M84" s="29"/>
-      <c r="N84" s="29"/>
+      <c r="L84" s="34"/>
+      <c r="M84" s="34"/>
+      <c r="N84" s="34"/>
     </row>
     <row r="85" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B85" s="35"/>
-      <c r="D85" s="28"/>
+      <c r="B85" s="40"/>
+      <c r="D85" s="33"/>
       <c r="E85" s="18"/>
       <c r="F85" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G85" s="46" t="s">
+      <c r="G85" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="H85" s="47"/>
-      <c r="I85" s="47" t="s">
+      <c r="H85" s="31"/>
+      <c r="I85" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="J85" s="46"/>
-      <c r="K85" s="46"/>
-      <c r="L85" s="29"/>
-      <c r="M85" s="29"/>
-      <c r="N85" s="29"/>
+      <c r="J85" s="30"/>
+      <c r="K85" s="30"/>
+      <c r="L85" s="34"/>
+      <c r="M85" s="34"/>
+      <c r="N85" s="34"/>
     </row>
     <row r="86" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B86" s="35"/>
-      <c r="D86" s="28"/>
+      <c r="B86" s="40"/>
+      <c r="D86" s="33"/>
       <c r="E86" s="17" t="s">
         <v>36</v>
       </c>
@@ -3277,13 +3304,13 @@
       <c r="K86" s="27">
         <v>0.17957555142145301</v>
       </c>
-      <c r="L86" s="29"/>
-      <c r="M86" s="29"/>
-      <c r="N86" s="29"/>
+      <c r="L86" s="34"/>
+      <c r="M86" s="34"/>
+      <c r="N86" s="34"/>
     </row>
     <row r="87" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B87" s="35"/>
-      <c r="D87" s="28"/>
+      <c r="B87" s="40"/>
+      <c r="D87" s="33"/>
       <c r="E87" s="18"/>
       <c r="F87" s="18" t="s">
         <v>23</v>
@@ -3303,33 +3330,39 @@
       <c r="K87" s="27">
         <v>18.97</v>
       </c>
-      <c r="L87" s="29"/>
-      <c r="M87" s="29"/>
-      <c r="N87" s="29"/>
+      <c r="L87" s="34"/>
+      <c r="M87" s="34"/>
+      <c r="N87" s="34"/>
     </row>
     <row r="88" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B88" s="35"/>
-      <c r="D88" s="28"/>
+      <c r="B88" s="40"/>
+      <c r="D88" s="33"/>
       <c r="E88" s="18"/>
       <c r="F88" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G88" s="46" t="s">
-        <v>124</v>
-      </c>
-      <c r="H88" s="47"/>
-      <c r="I88" s="47" t="s">
+      <c r="G88" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="H88" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I88" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="J88" s="46"/>
-      <c r="K88" s="46"/>
-      <c r="L88" s="29"/>
-      <c r="M88" s="29"/>
-      <c r="N88" s="29"/>
+      <c r="J88" s="27">
+        <v>0.248252583636414</v>
+      </c>
+      <c r="K88" s="27">
+        <v>0.21443854240184201</v>
+      </c>
+      <c r="L88" s="34"/>
+      <c r="M88" s="34"/>
+      <c r="N88" s="34"/>
     </row>
     <row r="89" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B89" s="35"/>
-      <c r="D89" s="28"/>
+      <c r="B89" s="40"/>
+      <c r="D89" s="33"/>
       <c r="E89" s="18"/>
       <c r="F89" s="18" t="s">
         <v>26</v>
@@ -3341,17 +3374,17 @@
       </c>
       <c r="J89" s="27"/>
       <c r="K89" s="27"/>
-      <c r="L89" s="29"/>
-      <c r="M89" s="29"/>
-      <c r="N89" s="29"/>
+      <c r="L89" s="34"/>
+      <c r="M89" s="34"/>
+      <c r="N89" s="34"/>
     </row>
     <row r="90" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B90" s="35"/>
-      <c r="G90" s="45"/>
+      <c r="B90" s="40"/>
+      <c r="G90" s="29"/>
     </row>
     <row r="91" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B91" s="35"/>
-      <c r="D91" s="28" t="s">
+      <c r="B91" s="40"/>
+      <c r="D91" s="33" t="s">
         <v>110</v>
       </c>
       <c r="E91" s="18" t="s">
@@ -3360,112 +3393,160 @@
       <c r="F91" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G91" s="26"/>
-      <c r="H91" s="18"/>
+      <c r="G91" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="H91" s="18" t="s">
+        <v>29</v>
+      </c>
       <c r="I91" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="J91" s="27"/>
-      <c r="K91" s="27"/>
-      <c r="L91" s="29"/>
-      <c r="M91" s="29"/>
-      <c r="N91" s="29"/>
+      <c r="J91" s="27">
+        <v>0.74119574703617896</v>
+      </c>
+      <c r="K91" s="27">
+        <v>0.73538087897381799</v>
+      </c>
+      <c r="L91" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="M91" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="N91" s="34">
+        <v>22136</v>
+      </c>
     </row>
     <row r="92" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B92" s="35"/>
-      <c r="D92" s="28"/>
+      <c r="B92" s="40"/>
+      <c r="D92" s="33"/>
       <c r="E92" s="18"/>
       <c r="F92" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G92" s="27"/>
-      <c r="H92" s="18"/>
+      <c r="G92" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="H92" s="32" t="s">
+        <v>16</v>
+      </c>
       <c r="I92" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="J92" s="27"/>
-      <c r="K92" s="27"/>
-      <c r="L92" s="29"/>
-      <c r="M92" s="29"/>
-      <c r="N92" s="29"/>
+      <c r="J92" s="27">
+        <v>0.75246800000000003</v>
+      </c>
+      <c r="K92" s="27">
+        <v>0.72577452283556598</v>
+      </c>
+      <c r="L92" s="34"/>
+      <c r="M92" s="34"/>
+      <c r="N92" s="34"/>
     </row>
     <row r="93" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B93" s="35"/>
-      <c r="D93" s="28"/>
+      <c r="B93" s="40"/>
+      <c r="D93" s="33"/>
       <c r="E93" s="18"/>
       <c r="F93" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G93" s="27"/>
-      <c r="H93" s="18"/>
-      <c r="I93" s="25" t="s">
+      <c r="G93" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="H93" s="31"/>
+      <c r="I93" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="J93" s="27"/>
-      <c r="K93" s="27"/>
-      <c r="L93" s="29"/>
-      <c r="M93" s="29"/>
-      <c r="N93" s="29"/>
+      <c r="J93" s="30"/>
+      <c r="K93" s="30"/>
+      <c r="L93" s="34"/>
+      <c r="M93" s="34"/>
+      <c r="N93" s="34"/>
     </row>
     <row r="94" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B94" s="35"/>
-      <c r="D94" s="28"/>
+      <c r="B94" s="40"/>
+      <c r="D94" s="33"/>
       <c r="E94" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F94" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G94" s="27"/>
-      <c r="H94" s="18"/>
+      <c r="G94" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="H94" s="32" t="s">
+        <v>24</v>
+      </c>
       <c r="I94" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="J94" s="27"/>
-      <c r="K94" s="27"/>
-      <c r="L94" s="29"/>
-      <c r="M94" s="29"/>
-      <c r="N94" s="29"/>
+      <c r="J94" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="K94" s="27">
+        <v>0.71784665775934897</v>
+      </c>
+      <c r="L94" s="34"/>
+      <c r="M94" s="34"/>
+      <c r="N94" s="34"/>
     </row>
     <row r="95" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B95" s="35"/>
-      <c r="D95" s="28"/>
+      <c r="B95" s="40"/>
+      <c r="D95" s="33"/>
       <c r="E95" s="18"/>
       <c r="F95" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G95" s="27"/>
-      <c r="H95" s="18"/>
+      <c r="G95" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="H95" s="32" t="s">
+        <v>24</v>
+      </c>
       <c r="I95" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="J95" s="27"/>
-      <c r="K95" s="27"/>
-      <c r="L95" s="29"/>
-      <c r="M95" s="29"/>
-      <c r="N95" s="29"/>
+      <c r="J95" s="27">
+        <v>95.403999999999996</v>
+      </c>
+      <c r="K95" s="27">
+        <v>68.430000000000007</v>
+      </c>
+      <c r="L95" s="34"/>
+      <c r="M95" s="34"/>
+      <c r="N95" s="34"/>
     </row>
     <row r="96" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B96" s="35"/>
-      <c r="D96" s="28"/>
+      <c r="B96" s="40"/>
+      <c r="D96" s="33"/>
       <c r="E96" s="18"/>
       <c r="F96" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G96" s="27"/>
-      <c r="H96" s="18"/>
+      <c r="G96" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="H96" s="32" t="s">
+        <v>76</v>
+      </c>
       <c r="I96" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="J96" s="27"/>
-      <c r="K96" s="27"/>
-      <c r="L96" s="29"/>
-      <c r="M96" s="29"/>
-      <c r="N96" s="29"/>
+      <c r="J96" s="27">
+        <v>0.75956174558959999</v>
+      </c>
+      <c r="K96" s="27">
+        <v>0.72422953987502703</v>
+      </c>
+      <c r="L96" s="34"/>
+      <c r="M96" s="34"/>
+      <c r="N96" s="34"/>
     </row>
     <row r="97" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B97" s="35"/>
-      <c r="D97" s="28"/>
+      <c r="B97" s="40"/>
+      <c r="D97" s="33"/>
       <c r="E97" s="18"/>
       <c r="F97" s="18" t="s">
         <v>26</v>
@@ -3477,9 +3558,9 @@
       </c>
       <c r="J97" s="27"/>
       <c r="K97" s="27"/>
-      <c r="L97" s="29"/>
-      <c r="M97" s="29"/>
-      <c r="N97" s="29"/>
+      <c r="L97" s="34"/>
+      <c r="M97" s="34"/>
+      <c r="N97" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="52">

</xml_diff>

<commit_message>
update resultados.xlsx (finished tests)
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="137">
   <si>
     <t>Ferramenta</t>
   </si>
@@ -395,9 +395,6 @@
   </si>
   <si>
     <t>4m18s</t>
-  </si>
-  <si>
-    <t>falta fazer</t>
   </si>
   <si>
     <t>Melhor: 0.2623</t>
@@ -460,18 +457,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -549,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -638,20 +629,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -659,44 +680,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -980,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D73" workbookViewId="0">
-      <selection activeCell="H89" sqref="H89"/>
+    <sheetView tabSelected="1" topLeftCell="B52" workbookViewId="0">
+      <selection activeCell="K88" sqref="K88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,13 +1061,13 @@
       <c r="K2" s="2">
         <v>2.3615173893038102</v>
       </c>
-      <c r="L2" s="42" t="s">
+      <c r="L2" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="M2" s="40" t="s">
+      <c r="M2" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="N2" s="40">
+      <c r="N2" s="34">
         <v>73</v>
       </c>
       <c r="R2" s="33" t="s">
@@ -1113,9 +1101,9 @@
       <c r="K3" s="2">
         <v>2.2556710599482699</v>
       </c>
-      <c r="L3" s="43"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
       <c r="R3" s="19" t="s">
         <v>2</v>
       </c>
@@ -1151,9 +1139,9 @@
       <c r="K4" s="2">
         <v>2.2502649752898698</v>
       </c>
-      <c r="L4" s="43"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
       <c r="R4" s="19" t="s">
         <v>3</v>
       </c>
@@ -1189,9 +1177,9 @@
       <c r="K5" s="7">
         <v>2.0563812623190301</v>
       </c>
-      <c r="L5" s="43"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
       <c r="R5" s="19" t="s">
         <v>28</v>
       </c>
@@ -1229,9 +1217,9 @@
       <c r="K6" s="4">
         <v>2.5263518439219701</v>
       </c>
-      <c r="L6" s="43"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
       <c r="R6" s="19" t="s">
         <v>38</v>
       </c>
@@ -1267,9 +1255,9 @@
       <c r="K7" s="2">
         <v>2.29</v>
       </c>
-      <c r="L7" s="43"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="40"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
       <c r="R7" s="19" t="s">
         <v>44</v>
       </c>
@@ -1305,9 +1293,9 @@
       <c r="K8" s="4">
         <v>2.0925560658435201</v>
       </c>
-      <c r="L8" s="43"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="40"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
       <c r="R8" s="19" t="s">
         <v>50</v>
       </c>
@@ -1323,7 +1311,7 @@
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B9" s="33"/>
-      <c r="D9" s="36"/>
+      <c r="D9" s="46"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8" t="s">
         <v>26</v>
@@ -1335,9 +1323,9 @@
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
       <c r="R9" s="19" t="s">
         <v>57</v>
       </c>
@@ -1379,7 +1367,7 @@
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B11" s="33"/>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="44" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="9" t="s">
@@ -1403,13 +1391,13 @@
       <c r="K11" s="16">
         <v>42.172544929804403</v>
       </c>
-      <c r="L11" s="45" t="s">
+      <c r="L11" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="M11" s="41" t="s">
+      <c r="M11" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="N11" s="41">
+      <c r="N11" s="48">
         <v>160</v>
       </c>
       <c r="R11" s="19" t="s">
@@ -1427,7 +1415,7 @@
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B12" s="33"/>
-      <c r="D12" s="38"/>
+      <c r="D12" s="35"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
         <v>15</v>
@@ -1447,9 +1435,9 @@
       <c r="K12" s="4">
         <v>42.4696075892439</v>
       </c>
-      <c r="L12" s="46"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
       <c r="R12" s="19" t="s">
         <v>103</v>
       </c>
@@ -1465,7 +1453,7 @@
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B13" s="33"/>
-      <c r="D13" s="38"/>
+      <c r="D13" s="35"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
         <v>17</v>
@@ -1485,9 +1473,9 @@
       <c r="K13" s="4">
         <v>43.043253511127602</v>
       </c>
-      <c r="L13" s="46"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="41"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
       <c r="R13" s="20" t="s">
         <v>108</v>
       </c>
@@ -1503,7 +1491,7 @@
     </row>
     <row r="14" spans="2:21" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="33"/>
-      <c r="D14" s="38"/>
+      <c r="D14" s="35"/>
       <c r="E14" s="5" t="s">
         <v>36</v>
       </c>
@@ -1525,9 +1513,9 @@
       <c r="K14" s="4">
         <v>42.455950916767499</v>
       </c>
-      <c r="L14" s="46"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="48"/>
       <c r="R14" s="20" t="s">
         <v>109</v>
       </c>
@@ -1543,7 +1531,7 @@
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B15" s="33"/>
-      <c r="D15" s="38"/>
+      <c r="D15" s="35"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4" t="s">
         <v>23</v>
@@ -1563,9 +1551,9 @@
       <c r="K15" s="4">
         <v>42.61</v>
       </c>
-      <c r="L15" s="46"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="41"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="48"/>
       <c r="R15" s="20" t="s">
         <v>110</v>
       </c>
@@ -1581,7 +1569,7 @@
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B16" s="33"/>
-      <c r="D16" s="38"/>
+      <c r="D16" s="35"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
         <v>25</v>
@@ -1601,13 +1589,13 @@
       <c r="K16" s="4">
         <v>42.954693127434403</v>
       </c>
-      <c r="L16" s="46"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="41"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="48"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="33"/>
-      <c r="D17" s="39"/>
+      <c r="D17" s="47"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8" t="s">
         <v>26</v>
@@ -1619,9 +1607,9 @@
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
-      <c r="L17" s="47"/>
-      <c r="M17" s="41"/>
-      <c r="N17" s="41"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="48"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="33"/>
@@ -1639,7 +1627,7 @@
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="33"/>
-      <c r="D19" s="37" t="s">
+      <c r="D19" s="44" t="s">
         <v>38</v>
       </c>
       <c r="E19" s="9" t="s">
@@ -1663,19 +1651,19 @@
       <c r="K19" s="9">
         <v>0.23469975874427401</v>
       </c>
-      <c r="L19" s="48" t="s">
+      <c r="L19" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="M19" s="34" t="s">
+      <c r="M19" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="N19" s="34">
+      <c r="N19" s="32">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="33"/>
-      <c r="D20" s="38"/>
+      <c r="D20" s="35"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
         <v>15</v>
@@ -1695,13 +1683,13 @@
       <c r="K20" s="4">
         <v>0.26615681314328199</v>
       </c>
-      <c r="L20" s="49"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="32"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="33"/>
-      <c r="D21" s="38"/>
+      <c r="D21" s="35"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
         <v>17</v>
@@ -1721,13 +1709,13 @@
       <c r="K21" s="4">
         <v>0.27054514227366</v>
       </c>
-      <c r="L21" s="49"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
     </row>
     <row r="22" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="33"/>
-      <c r="D22" s="38"/>
+      <c r="D22" s="35"/>
       <c r="E22" s="5" t="s">
         <v>36</v>
       </c>
@@ -1749,13 +1737,13 @@
       <c r="K22" s="7">
         <v>0.23440350034482499</v>
       </c>
-      <c r="L22" s="49"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="33"/>
-      <c r="D23" s="38"/>
+      <c r="D23" s="35"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4" t="s">
         <v>23</v>
@@ -1775,13 +1763,13 @@
       <c r="K23" s="4">
         <v>0.27</v>
       </c>
-      <c r="L23" s="49"/>
-      <c r="M23" s="34"/>
-      <c r="N23" s="34"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="32"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="33"/>
-      <c r="D24" s="38"/>
+      <c r="D24" s="35"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4" t="s">
         <v>25</v>
@@ -1801,13 +1789,13 @@
       <c r="K24" s="4">
         <v>0.24189871737548899</v>
       </c>
-      <c r="L24" s="49"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
+      <c r="L24" s="43"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="32"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="33"/>
-      <c r="D25" s="39"/>
+      <c r="D25" s="47"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8" t="s">
         <v>26</v>
@@ -1819,9 +1807,9 @@
       </c>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
-      <c r="L25" s="37"/>
-      <c r="M25" s="34"/>
-      <c r="N25" s="34"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="33"/>
@@ -1839,7 +1827,7 @@
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="33"/>
-      <c r="D27" s="37" t="s">
+      <c r="D27" s="44" t="s">
         <v>45</v>
       </c>
       <c r="E27" s="9" t="s">
@@ -1863,19 +1851,19 @@
       <c r="K27" s="9">
         <v>141.96334027640401</v>
       </c>
-      <c r="L27" s="48" t="s">
+      <c r="L27" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="M27" s="34" t="s">
+      <c r="M27" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="N27" s="34">
+      <c r="N27" s="32">
         <v>15</v>
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="33"/>
-      <c r="D28" s="38"/>
+      <c r="D28" s="35"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4" t="s">
         <v>15</v>
@@ -1895,13 +1883,13 @@
       <c r="K28" s="4">
         <v>146.72373452591</v>
       </c>
-      <c r="L28" s="49"/>
-      <c r="M28" s="34"/>
-      <c r="N28" s="34"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="32"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="33"/>
-      <c r="D29" s="38"/>
+      <c r="D29" s="35"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4" t="s">
         <v>17</v>
@@ -1921,13 +1909,13 @@
       <c r="K29" s="7">
         <v>140.69022615456799</v>
       </c>
-      <c r="L29" s="49"/>
-      <c r="M29" s="34"/>
-      <c r="N29" s="34"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="32"/>
+      <c r="N29" s="32"/>
     </row>
     <row r="30" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="33"/>
-      <c r="D30" s="38"/>
+      <c r="D30" s="35"/>
       <c r="E30" s="5" t="s">
         <v>36</v>
       </c>
@@ -1949,13 +1937,13 @@
       <c r="K30" s="4">
         <v>142.52852874723999</v>
       </c>
-      <c r="L30" s="49"/>
-      <c r="M30" s="34"/>
-      <c r="N30" s="34"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="32"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="33"/>
-      <c r="D31" s="38"/>
+      <c r="D31" s="35"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4" t="s">
         <v>23</v>
@@ -1975,13 +1963,13 @@
       <c r="K31" s="4">
         <v>152.29</v>
       </c>
-      <c r="L31" s="49"/>
-      <c r="M31" s="34"/>
-      <c r="N31" s="34"/>
+      <c r="L31" s="43"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="32"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="33"/>
-      <c r="D32" s="38"/>
+      <c r="D32" s="35"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4" t="s">
         <v>25</v>
@@ -2001,13 +1989,13 @@
       <c r="K32" s="4">
         <v>144.833568734441</v>
       </c>
-      <c r="L32" s="49"/>
-      <c r="M32" s="34"/>
-      <c r="N32" s="34"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="32"/>
+      <c r="N32" s="32"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="33"/>
-      <c r="D33" s="39"/>
+      <c r="D33" s="47"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8" t="s">
         <v>26</v>
@@ -2019,9 +2007,9 @@
       </c>
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="34"/>
-      <c r="N33" s="34"/>
+      <c r="L33" s="44"/>
+      <c r="M33" s="32"/>
+      <c r="N33" s="32"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D34" s="13"/>
@@ -2037,10 +2025,10 @@
       <c r="N34" s="11"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="40" t="s">
+      <c r="B35" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="35" t="s">
+      <c r="D35" s="45" t="s">
         <v>50</v>
       </c>
       <c r="E35" s="9" t="s">
@@ -2064,18 +2052,18 @@
       <c r="K35" s="9">
         <v>0.910468209203948</v>
       </c>
-      <c r="L35" s="48" t="s">
+      <c r="L35" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="M35" s="34" t="s">
+      <c r="M35" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="N35" s="34">
+      <c r="N35" s="32">
         <v>5132</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B36" s="40"/>
+      <c r="B36" s="34"/>
       <c r="D36" s="33"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4" t="s">
@@ -2096,12 +2084,12 @@
       <c r="K36" s="4">
         <v>0.88615775755244997</v>
       </c>
-      <c r="L36" s="49"/>
-      <c r="M36" s="34"/>
-      <c r="N36" s="34"/>
+      <c r="L36" s="43"/>
+      <c r="M36" s="32"/>
+      <c r="N36" s="32"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="40"/>
+      <c r="B37" s="34"/>
       <c r="D37" s="33"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4" t="s">
@@ -2122,12 +2110,12 @@
       <c r="K37" s="4">
         <v>0.87077511430158505</v>
       </c>
-      <c r="L37" s="49"/>
-      <c r="M37" s="34"/>
-      <c r="N37" s="34"/>
+      <c r="L37" s="43"/>
+      <c r="M37" s="32"/>
+      <c r="N37" s="32"/>
     </row>
     <row r="38" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B38" s="40"/>
+      <c r="B38" s="34"/>
       <c r="D38" s="33"/>
       <c r="E38" s="5" t="s">
         <v>36</v>
@@ -2150,12 +2138,12 @@
       <c r="K38" s="4">
         <v>0.91063111566893096</v>
       </c>
-      <c r="L38" s="49"/>
-      <c r="M38" s="34"/>
-      <c r="N38" s="34"/>
+      <c r="L38" s="43"/>
+      <c r="M38" s="32"/>
+      <c r="N38" s="32"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B39" s="40"/>
+      <c r="B39" s="34"/>
       <c r="D39" s="33"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4" t="s">
@@ -2176,12 +2164,12 @@
       <c r="K39" s="4">
         <v>0.91</v>
       </c>
-      <c r="L39" s="49"/>
-      <c r="M39" s="34"/>
-      <c r="N39" s="34"/>
+      <c r="L39" s="43"/>
+      <c r="M39" s="32"/>
+      <c r="N39" s="32"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B40" s="40"/>
+      <c r="B40" s="34"/>
       <c r="D40" s="33"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4" t="s">
@@ -2202,13 +2190,13 @@
       <c r="K40" s="7">
         <v>0.91188896722642299</v>
       </c>
-      <c r="L40" s="49"/>
-      <c r="M40" s="34"/>
-      <c r="N40" s="34"/>
+      <c r="L40" s="43"/>
+      <c r="M40" s="32"/>
+      <c r="N40" s="32"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B41" s="40"/>
-      <c r="D41" s="36"/>
+      <c r="B41" s="34"/>
+      <c r="D41" s="46"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8" t="s">
         <v>26</v>
@@ -2220,12 +2208,12 @@
       </c>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
-      <c r="L41" s="37"/>
-      <c r="M41" s="34"/>
-      <c r="N41" s="34"/>
+      <c r="L41" s="44"/>
+      <c r="M41" s="32"/>
+      <c r="N41" s="32"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B42" s="40"/>
+      <c r="B42" s="34"/>
       <c r="D42" s="12"/>
       <c r="E42" s="13"/>
       <c r="F42" s="13"/>
@@ -2239,8 +2227,8 @@
       <c r="N42" s="11"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B43" s="40"/>
-      <c r="D43" s="35" t="s">
+      <c r="B43" s="34"/>
+      <c r="D43" s="45" t="s">
         <v>57</v>
       </c>
       <c r="E43" s="9" t="s">
@@ -2264,18 +2252,18 @@
       <c r="K43" s="9">
         <v>0.78503433208489304</v>
       </c>
-      <c r="L43" s="34" t="s">
+      <c r="L43" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="M43" s="34" t="s">
+      <c r="M43" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="N43" s="34">
+      <c r="N43" s="32">
         <v>419021</v>
       </c>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B44" s="40"/>
+      <c r="B44" s="34"/>
       <c r="D44" s="33"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4" t="s">
@@ -2296,12 +2284,12 @@
       <c r="K44" s="4">
         <v>0.59706616729088602</v>
       </c>
-      <c r="L44" s="38"/>
-      <c r="M44" s="34"/>
-      <c r="N44" s="34"/>
+      <c r="L44" s="35"/>
+      <c r="M44" s="32"/>
+      <c r="N44" s="32"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B45" s="40"/>
+      <c r="B45" s="34"/>
       <c r="D45" s="33"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4" t="s">
@@ -2322,12 +2310,12 @@
       <c r="K45" s="4">
         <v>0.71168851435705305</v>
       </c>
-      <c r="L45" s="38"/>
-      <c r="M45" s="34"/>
-      <c r="N45" s="34"/>
+      <c r="L45" s="35"/>
+      <c r="M45" s="32"/>
+      <c r="N45" s="32"/>
     </row>
     <row r="46" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B46" s="40"/>
+      <c r="B46" s="34"/>
       <c r="D46" s="33"/>
       <c r="E46" s="5" t="s">
         <v>36</v>
@@ -2350,12 +2338,12 @@
       <c r="K46" s="4">
         <v>0.77699750312109805</v>
       </c>
-      <c r="L46" s="38"/>
-      <c r="M46" s="34"/>
-      <c r="N46" s="34"/>
+      <c r="L46" s="35"/>
+      <c r="M46" s="32"/>
+      <c r="N46" s="32"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B47" s="40"/>
+      <c r="B47" s="34"/>
       <c r="D47" s="33"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4" t="s">
@@ -2376,12 +2364,12 @@
       <c r="K47" s="7">
         <v>0.8</v>
       </c>
-      <c r="L47" s="38"/>
-      <c r="M47" s="34"/>
-      <c r="N47" s="34"/>
+      <c r="L47" s="35"/>
+      <c r="M47" s="32"/>
+      <c r="N47" s="32"/>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B48" s="40"/>
+      <c r="B48" s="34"/>
       <c r="D48" s="33"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4" t="s">
@@ -2402,13 +2390,13 @@
       <c r="K48" s="7">
         <v>0.80024968789013695</v>
       </c>
-      <c r="L48" s="38"/>
-      <c r="M48" s="34"/>
-      <c r="N48" s="34"/>
+      <c r="L48" s="35"/>
+      <c r="M48" s="32"/>
+      <c r="N48" s="32"/>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B49" s="40"/>
-      <c r="D49" s="36"/>
+      <c r="B49" s="34"/>
+      <c r="D49" s="46"/>
       <c r="E49" s="8"/>
       <c r="F49" s="8" t="s">
         <v>26</v>
@@ -2420,12 +2408,12 @@
       </c>
       <c r="J49" s="8"/>
       <c r="K49" s="8"/>
-      <c r="L49" s="38"/>
-      <c r="M49" s="34"/>
-      <c r="N49" s="34"/>
+      <c r="L49" s="35"/>
+      <c r="M49" s="32"/>
+      <c r="N49" s="32"/>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B50" s="40"/>
+      <c r="B50" s="34"/>
       <c r="D50" s="12"/>
       <c r="E50" s="13"/>
       <c r="F50" s="13"/>
@@ -2439,8 +2427,8 @@
       <c r="N50" s="11"/>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B51" s="40"/>
-      <c r="D51" s="35" t="s">
+      <c r="B51" s="34"/>
+      <c r="D51" s="45" t="s">
         <v>62</v>
       </c>
       <c r="E51" s="9" t="s">
@@ -2464,18 +2452,18 @@
       <c r="K51" s="9">
         <v>0.94655497110201903</v>
       </c>
-      <c r="L51" s="34" t="s">
+      <c r="L51" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="M51" s="34" t="s">
+      <c r="M51" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="N51" s="34">
+      <c r="N51" s="32">
         <v>147659</v>
       </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B52" s="40"/>
+      <c r="B52" s="34"/>
       <c r="D52" s="33"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4" t="s">
@@ -2496,12 +2484,12 @@
       <c r="K52" s="4">
         <v>0.83995714007403</v>
       </c>
-      <c r="L52" s="38"/>
-      <c r="M52" s="34"/>
-      <c r="N52" s="34"/>
+      <c r="L52" s="35"/>
+      <c r="M52" s="32"/>
+      <c r="N52" s="32"/>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B53" s="40"/>
+      <c r="B53" s="34"/>
       <c r="D53" s="33"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4" t="s">
@@ -2522,12 +2510,12 @@
       <c r="K53" s="7">
         <v>1</v>
       </c>
-      <c r="L53" s="38"/>
-      <c r="M53" s="34"/>
-      <c r="N53" s="34"/>
+      <c r="L53" s="35"/>
+      <c r="M53" s="32"/>
+      <c r="N53" s="32"/>
     </row>
     <row r="54" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B54" s="40"/>
+      <c r="B54" s="34"/>
       <c r="D54" s="33"/>
       <c r="E54" s="5" t="s">
         <v>36</v>
@@ -2550,12 +2538,12 @@
       <c r="K54" s="4">
         <v>0.97873848082154702</v>
       </c>
-      <c r="L54" s="38"/>
-      <c r="M54" s="34"/>
-      <c r="N54" s="34"/>
+      <c r="L54" s="35"/>
+      <c r="M54" s="32"/>
+      <c r="N54" s="32"/>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B55" s="40"/>
+      <c r="B55" s="34"/>
       <c r="D55" s="33"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4" t="s">
@@ -2576,12 +2564,12 @@
       <c r="K55" s="4">
         <v>0.94</v>
       </c>
-      <c r="L55" s="38"/>
-      <c r="M55" s="34"/>
-      <c r="N55" s="34"/>
+      <c r="L55" s="35"/>
+      <c r="M55" s="32"/>
+      <c r="N55" s="32"/>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B56" s="40"/>
+      <c r="B56" s="34"/>
       <c r="D56" s="33"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4" t="s">
@@ -2602,13 +2590,13 @@
       <c r="K56" s="7">
         <v>1</v>
       </c>
-      <c r="L56" s="38"/>
-      <c r="M56" s="34"/>
-      <c r="N56" s="34"/>
+      <c r="L56" s="35"/>
+      <c r="M56" s="32"/>
+      <c r="N56" s="32"/>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B57" s="40"/>
-      <c r="D57" s="36"/>
+      <c r="B57" s="34"/>
+      <c r="D57" s="46"/>
       <c r="E57" s="8"/>
       <c r="F57" s="8" t="s">
         <v>26</v>
@@ -2620,12 +2608,12 @@
       </c>
       <c r="J57" s="8"/>
       <c r="K57" s="8"/>
-      <c r="L57" s="38"/>
-      <c r="M57" s="34"/>
-      <c r="N57" s="34"/>
+      <c r="L57" s="35"/>
+      <c r="M57" s="32"/>
+      <c r="N57" s="32"/>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B58" s="40"/>
+      <c r="B58" s="34"/>
       <c r="D58" s="12"/>
       <c r="E58" s="13"/>
       <c r="F58" s="13"/>
@@ -2639,7 +2627,7 @@
       <c r="N58" s="11"/>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B59" s="40"/>
+      <c r="B59" s="34"/>
       <c r="D59" s="33" t="s">
         <v>103</v>
       </c>
@@ -2664,18 +2652,18 @@
       <c r="K59" s="27">
         <v>0.80959113938965399</v>
       </c>
-      <c r="L59" s="34" t="s">
+      <c r="L59" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="M59" s="34" t="s">
+      <c r="M59" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="N59" s="34">
+      <c r="N59" s="32">
         <v>132164</v>
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B60" s="40"/>
+      <c r="B60" s="34"/>
       <c r="D60" s="33"/>
       <c r="E60" s="18"/>
       <c r="F60" s="18" t="s">
@@ -2696,12 +2684,12 @@
       <c r="K60" s="27">
         <v>0.72940968540120099</v>
       </c>
-      <c r="L60" s="34"/>
-      <c r="M60" s="34"/>
-      <c r="N60" s="34"/>
+      <c r="L60" s="32"/>
+      <c r="M60" s="32"/>
+      <c r="N60" s="32"/>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B61" s="40"/>
+      <c r="B61" s="34"/>
       <c r="D61" s="33"/>
       <c r="E61" s="18"/>
       <c r="F61" s="18" t="s">
@@ -2722,12 +2710,12 @@
       <c r="K61" s="27">
         <v>0.65676917638741605</v>
       </c>
-      <c r="L61" s="34"/>
-      <c r="M61" s="34"/>
-      <c r="N61" s="34"/>
+      <c r="L61" s="32"/>
+      <c r="M61" s="32"/>
+      <c r="N61" s="32"/>
     </row>
     <row r="62" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B62" s="40"/>
+      <c r="B62" s="34"/>
       <c r="D62" s="33"/>
       <c r="E62" s="17" t="s">
         <v>36</v>
@@ -2750,12 +2738,12 @@
       <c r="K62" s="27">
         <v>0.81654294803817595</v>
       </c>
-      <c r="L62" s="34"/>
-      <c r="M62" s="34"/>
-      <c r="N62" s="34"/>
+      <c r="L62" s="32"/>
+      <c r="M62" s="32"/>
+      <c r="N62" s="32"/>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B63" s="40"/>
+      <c r="B63" s="34"/>
       <c r="D63" s="33"/>
       <c r="E63" s="18"/>
       <c r="F63" s="18" t="s">
@@ -2776,12 +2764,12 @@
       <c r="K63" s="27">
         <v>0.81</v>
       </c>
-      <c r="L63" s="34"/>
-      <c r="M63" s="34"/>
-      <c r="N63" s="34"/>
+      <c r="L63" s="32"/>
+      <c r="M63" s="32"/>
+      <c r="N63" s="32"/>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B64" s="40"/>
+      <c r="B64" s="34"/>
       <c r="D64" s="33"/>
       <c r="E64" s="18"/>
       <c r="F64" s="18" t="s">
@@ -2802,12 +2790,12 @@
       <c r="K64" s="27">
         <v>0.80452456698480002</v>
       </c>
-      <c r="L64" s="34"/>
-      <c r="M64" s="34"/>
-      <c r="N64" s="34"/>
+      <c r="L64" s="32"/>
+      <c r="M64" s="32"/>
+      <c r="N64" s="32"/>
     </row>
     <row r="65" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B65" s="40"/>
+      <c r="B65" s="34"/>
       <c r="D65" s="33"/>
       <c r="E65" s="18"/>
       <c r="F65" s="18" t="s">
@@ -2820,12 +2808,12 @@
       </c>
       <c r="J65" s="27"/>
       <c r="K65" s="27"/>
-      <c r="L65" s="34"/>
-      <c r="M65" s="34"/>
-      <c r="N65" s="34"/>
+      <c r="L65" s="32"/>
+      <c r="M65" s="32"/>
+      <c r="N65" s="32"/>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B67" s="40" t="s">
+      <c r="B67" s="34" t="s">
         <v>106</v>
       </c>
       <c r="D67" s="33" t="s">
@@ -2852,18 +2840,18 @@
       <c r="K67" s="18">
         <v>0.81557623894257503</v>
       </c>
-      <c r="L67" s="34" t="s">
+      <c r="L67" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="M67" s="34" t="s">
+      <c r="M67" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="N67" s="34">
+      <c r="N67" s="32">
         <v>23532</v>
       </c>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B68" s="40"/>
+      <c r="B68" s="34"/>
       <c r="D68" s="33"/>
       <c r="E68" s="18"/>
       <c r="F68" s="18" t="s">
@@ -2884,12 +2872,12 @@
       <c r="K68" s="18">
         <v>0.88222010940682705</v>
       </c>
-      <c r="L68" s="34"/>
-      <c r="M68" s="34"/>
-      <c r="N68" s="34"/>
+      <c r="L68" s="32"/>
+      <c r="M68" s="32"/>
+      <c r="N68" s="32"/>
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B69" s="40"/>
+      <c r="B69" s="34"/>
       <c r="D69" s="33"/>
       <c r="E69" s="18"/>
       <c r="F69" s="18" t="s">
@@ -2910,12 +2898,12 @@
       <c r="K69" s="18">
         <v>0.84568164621720798</v>
       </c>
-      <c r="L69" s="34"/>
-      <c r="M69" s="34"/>
-      <c r="N69" s="34"/>
+      <c r="L69" s="32"/>
+      <c r="M69" s="32"/>
+      <c r="N69" s="32"/>
     </row>
     <row r="70" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B70" s="40"/>
+      <c r="B70" s="34"/>
       <c r="D70" s="33"/>
       <c r="E70" s="17" t="s">
         <v>36</v>
@@ -2938,12 +2926,12 @@
       <c r="K70" s="18">
         <v>0.80867398669225798</v>
       </c>
-      <c r="L70" s="34"/>
-      <c r="M70" s="34"/>
-      <c r="N70" s="34"/>
+      <c r="L70" s="32"/>
+      <c r="M70" s="32"/>
+      <c r="N70" s="32"/>
     </row>
     <row r="71" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B71" s="40"/>
+      <c r="B71" s="34"/>
       <c r="D71" s="33"/>
       <c r="E71" s="18"/>
       <c r="F71" s="18" t="s">
@@ -2964,12 +2952,12 @@
       <c r="K71" s="7">
         <v>1</v>
       </c>
-      <c r="L71" s="34"/>
-      <c r="M71" s="34"/>
-      <c r="N71" s="34"/>
+      <c r="L71" s="32"/>
+      <c r="M71" s="32"/>
+      <c r="N71" s="32"/>
     </row>
     <row r="72" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B72" s="40"/>
+      <c r="B72" s="34"/>
       <c r="D72" s="33"/>
       <c r="E72" s="18"/>
       <c r="F72" s="18" t="s">
@@ -2990,12 +2978,12 @@
       <c r="K72" s="18">
         <v>0.75754008756888402</v>
       </c>
-      <c r="L72" s="34"/>
-      <c r="M72" s="34"/>
-      <c r="N72" s="34"/>
+      <c r="L72" s="32"/>
+      <c r="M72" s="32"/>
+      <c r="N72" s="32"/>
     </row>
     <row r="73" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B73" s="40"/>
+      <c r="B73" s="34"/>
       <c r="D73" s="33"/>
       <c r="E73" s="18"/>
       <c r="F73" s="18" t="s">
@@ -3008,15 +2996,15 @@
       </c>
       <c r="J73" s="18"/>
       <c r="K73" s="18"/>
-      <c r="L73" s="34"/>
-      <c r="M73" s="34"/>
-      <c r="N73" s="34"/>
+      <c r="L73" s="32"/>
+      <c r="M73" s="32"/>
+      <c r="N73" s="32"/>
     </row>
     <row r="74" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B74" s="40"/>
+      <c r="B74" s="34"/>
     </row>
     <row r="75" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B75" s="40"/>
+      <c r="B75" s="34"/>
       <c r="D75" s="33" t="s">
         <v>108</v>
       </c>
@@ -3041,18 +3029,18 @@
       <c r="K75" s="27">
         <v>0.55025061075102</v>
       </c>
-      <c r="L75" s="34" t="s">
+      <c r="L75" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="M75" s="34" t="s">
+      <c r="M75" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="N75" s="34">
+      <c r="N75" s="32">
         <v>21446</v>
       </c>
     </row>
     <row r="76" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B76" s="40"/>
+      <c r="B76" s="34"/>
       <c r="D76" s="33"/>
       <c r="E76" s="18"/>
       <c r="F76" s="18" t="s">
@@ -3073,32 +3061,38 @@
       <c r="K76" s="27">
         <v>0.55299548558353595</v>
       </c>
-      <c r="L76" s="34"/>
-      <c r="M76" s="34"/>
-      <c r="N76" s="34"/>
+      <c r="L76" s="32"/>
+      <c r="M76" s="32"/>
+      <c r="N76" s="32"/>
     </row>
     <row r="77" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B77" s="40"/>
+      <c r="B77" s="34"/>
       <c r="D77" s="33"/>
       <c r="E77" s="18"/>
       <c r="F77" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G77" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="H77" s="31"/>
+      <c r="G77" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="H77" s="31" t="s">
+        <v>18</v>
+      </c>
       <c r="I77" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="J77" s="30"/>
-      <c r="K77" s="30"/>
-      <c r="L77" s="34"/>
-      <c r="M77" s="34"/>
-      <c r="N77" s="34"/>
+      <c r="J77" s="27">
+        <v>0.55411299999999997</v>
+      </c>
+      <c r="K77" s="7">
+        <v>0.57296936343814298</v>
+      </c>
+      <c r="L77" s="32"/>
+      <c r="M77" s="32"/>
+      <c r="N77" s="32"/>
     </row>
     <row r="78" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B78" s="40"/>
+      <c r="B78" s="34"/>
       <c r="D78" s="33"/>
       <c r="E78" s="17" t="s">
         <v>36</v>
@@ -3121,12 +3115,12 @@
       <c r="K78" s="27">
         <v>0.52849268592134702</v>
       </c>
-      <c r="L78" s="34"/>
-      <c r="M78" s="34"/>
-      <c r="N78" s="34"/>
+      <c r="L78" s="32"/>
+      <c r="M78" s="32"/>
+      <c r="N78" s="32"/>
     </row>
     <row r="79" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B79" s="40"/>
+      <c r="B79" s="34"/>
       <c r="D79" s="33"/>
       <c r="E79" s="18"/>
       <c r="F79" s="18" t="s">
@@ -3147,12 +3141,12 @@
       <c r="K79" s="27">
         <v>0.49690000000000001</v>
       </c>
-      <c r="L79" s="34"/>
-      <c r="M79" s="34"/>
-      <c r="N79" s="34"/>
+      <c r="L79" s="32"/>
+      <c r="M79" s="32"/>
+      <c r="N79" s="32"/>
     </row>
     <row r="80" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B80" s="40"/>
+      <c r="B80" s="34"/>
       <c r="D80" s="33"/>
       <c r="E80" s="18"/>
       <c r="F80" s="18" t="s">
@@ -3173,12 +3167,12 @@
       <c r="K80" s="27">
         <v>0.56739713139489401</v>
       </c>
-      <c r="L80" s="34"/>
-      <c r="M80" s="34"/>
-      <c r="N80" s="34"/>
+      <c r="L80" s="32"/>
+      <c r="M80" s="32"/>
+      <c r="N80" s="32"/>
     </row>
     <row r="81" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B81" s="40"/>
+      <c r="B81" s="34"/>
       <c r="D81" s="33"/>
       <c r="E81" s="18"/>
       <c r="F81" s="18" t="s">
@@ -3191,15 +3185,15 @@
       </c>
       <c r="J81" s="27"/>
       <c r="K81" s="27"/>
-      <c r="L81" s="34"/>
-      <c r="M81" s="34"/>
-      <c r="N81" s="34"/>
+      <c r="L81" s="32"/>
+      <c r="M81" s="32"/>
+      <c r="N81" s="32"/>
     </row>
     <row r="82" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B82" s="40"/>
+      <c r="B82" s="34"/>
     </row>
     <row r="83" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B83" s="40"/>
+      <c r="B83" s="34"/>
       <c r="D83" s="33" t="s">
         <v>109</v>
       </c>
@@ -3210,7 +3204,7 @@
         <v>1</v>
       </c>
       <c r="G83" s="26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H83" s="18" t="s">
         <v>53</v>
@@ -3224,28 +3218,28 @@
       <c r="K83" s="27">
         <v>0.213985952346849</v>
       </c>
-      <c r="L83" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="M83" s="34" t="s">
+      <c r="L83" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="M83" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="N83" s="34">
+      <c r="N83" s="32">
         <v>19445</v>
       </c>
     </row>
     <row r="84" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B84" s="40"/>
+      <c r="B84" s="34"/>
       <c r="D84" s="33"/>
       <c r="E84" s="18"/>
       <c r="F84" s="18" t="s">
         <v>15</v>
       </c>
       <c r="G84" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="H84" s="25" t="s">
         <v>127</v>
-      </c>
-      <c r="H84" s="25" t="s">
-        <v>128</v>
       </c>
       <c r="I84" s="25" t="s">
         <v>70</v>
@@ -3256,32 +3250,38 @@
       <c r="K84" s="27">
         <v>0.181546683325744</v>
       </c>
-      <c r="L84" s="34"/>
-      <c r="M84" s="34"/>
-      <c r="N84" s="34"/>
+      <c r="L84" s="32"/>
+      <c r="M84" s="32"/>
+      <c r="N84" s="32"/>
     </row>
     <row r="85" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B85" s="40"/>
+      <c r="B85" s="34"/>
       <c r="D85" s="33"/>
       <c r="E85" s="18"/>
       <c r="F85" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G85" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="H85" s="31"/>
+      <c r="G85" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="H85" s="31" t="s">
+        <v>18</v>
+      </c>
       <c r="I85" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="J85" s="30"/>
-      <c r="K85" s="30"/>
-      <c r="L85" s="34"/>
-      <c r="M85" s="34"/>
-      <c r="N85" s="34"/>
+      <c r="J85" s="27">
+        <v>0.237265</v>
+      </c>
+      <c r="K85" s="27">
+        <v>0.176738765308842</v>
+      </c>
+      <c r="L85" s="32"/>
+      <c r="M85" s="32"/>
+      <c r="N85" s="32"/>
     </row>
     <row r="86" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B86" s="40"/>
+      <c r="B86" s="34"/>
       <c r="D86" s="33"/>
       <c r="E86" s="17" t="s">
         <v>36</v>
@@ -3290,7 +3290,7 @@
         <v>21</v>
       </c>
       <c r="G86" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H86" s="25" t="s">
         <v>24</v>
@@ -3304,19 +3304,19 @@
       <c r="K86" s="27">
         <v>0.17957555142145301</v>
       </c>
-      <c r="L86" s="34"/>
-      <c r="M86" s="34"/>
-      <c r="N86" s="34"/>
+      <c r="L86" s="32"/>
+      <c r="M86" s="32"/>
+      <c r="N86" s="32"/>
     </row>
     <row r="87" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B87" s="40"/>
+      <c r="B87" s="34"/>
       <c r="D87" s="33"/>
       <c r="E87" s="18"/>
       <c r="F87" s="18" t="s">
         <v>23</v>
       </c>
       <c r="G87" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H87" s="25" t="s">
         <v>24</v>
@@ -3330,19 +3330,19 @@
       <c r="K87" s="27">
         <v>18.97</v>
       </c>
-      <c r="L87" s="34"/>
-      <c r="M87" s="34"/>
-      <c r="N87" s="34"/>
+      <c r="L87" s="32"/>
+      <c r="M87" s="32"/>
+      <c r="N87" s="32"/>
     </row>
     <row r="88" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B88" s="40"/>
+      <c r="B88" s="34"/>
       <c r="D88" s="33"/>
       <c r="E88" s="18"/>
       <c r="F88" s="18" t="s">
         <v>25</v>
       </c>
       <c r="G88" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H88" s="28" t="s">
         <v>80</v>
@@ -3353,15 +3353,15 @@
       <c r="J88" s="27">
         <v>0.248252583636414</v>
       </c>
-      <c r="K88" s="27">
+      <c r="K88" s="7">
         <v>0.21443854240184201</v>
       </c>
-      <c r="L88" s="34"/>
-      <c r="M88" s="34"/>
-      <c r="N88" s="34"/>
+      <c r="L88" s="32"/>
+      <c r="M88" s="32"/>
+      <c r="N88" s="32"/>
     </row>
     <row r="89" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B89" s="40"/>
+      <c r="B89" s="34"/>
       <c r="D89" s="33"/>
       <c r="E89" s="18"/>
       <c r="F89" s="18" t="s">
@@ -3374,16 +3374,16 @@
       </c>
       <c r="J89" s="27"/>
       <c r="K89" s="27"/>
-      <c r="L89" s="34"/>
-      <c r="M89" s="34"/>
-      <c r="N89" s="34"/>
+      <c r="L89" s="32"/>
+      <c r="M89" s="32"/>
+      <c r="N89" s="32"/>
     </row>
     <row r="90" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B90" s="40"/>
+      <c r="B90" s="34"/>
       <c r="G90" s="29"/>
     </row>
     <row r="91" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B91" s="40"/>
+      <c r="B91" s="34"/>
       <c r="D91" s="33" t="s">
         <v>110</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>1</v>
       </c>
       <c r="G91" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H91" s="18" t="s">
         <v>29</v>
@@ -3405,30 +3405,30 @@
       <c r="J91" s="27">
         <v>0.74119574703617896</v>
       </c>
-      <c r="K91" s="27">
+      <c r="K91" s="7">
         <v>0.73538087897381799</v>
       </c>
-      <c r="L91" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="M91" s="34" t="s">
+      <c r="L91" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="M91" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="N91" s="34">
+      <c r="N91" s="32">
         <v>22136</v>
       </c>
     </row>
     <row r="92" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B92" s="40"/>
+      <c r="B92" s="34"/>
       <c r="D92" s="33"/>
       <c r="E92" s="18"/>
       <c r="F92" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G92" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="H92" s="32" t="s">
+      <c r="G92" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="H92" s="30" t="s">
         <v>16</v>
       </c>
       <c r="I92" s="25" t="s">
@@ -3440,32 +3440,38 @@
       <c r="K92" s="27">
         <v>0.72577452283556598</v>
       </c>
-      <c r="L92" s="34"/>
-      <c r="M92" s="34"/>
-      <c r="N92" s="34"/>
+      <c r="L92" s="32"/>
+      <c r="M92" s="32"/>
+      <c r="N92" s="32"/>
     </row>
     <row r="93" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B93" s="40"/>
+      <c r="B93" s="34"/>
       <c r="D93" s="33"/>
       <c r="E93" s="18"/>
       <c r="F93" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G93" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="H93" s="31"/>
+      <c r="G93" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="H93" s="31" t="s">
+        <v>18</v>
+      </c>
       <c r="I93" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="J93" s="30"/>
-      <c r="K93" s="30"/>
-      <c r="L93" s="34"/>
-      <c r="M93" s="34"/>
-      <c r="N93" s="34"/>
+      <c r="J93" s="27">
+        <v>0.75241999999999998</v>
+      </c>
+      <c r="K93" s="27">
+        <v>0.72230513333245805</v>
+      </c>
+      <c r="L93" s="32"/>
+      <c r="M93" s="32"/>
+      <c r="N93" s="32"/>
     </row>
     <row r="94" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B94" s="40"/>
+      <c r="B94" s="34"/>
       <c r="D94" s="33"/>
       <c r="E94" s="17" t="s">
         <v>36</v>
@@ -3474,35 +3480,35 @@
         <v>21</v>
       </c>
       <c r="G94" s="27" t="s">
-        <v>136</v>
-      </c>
-      <c r="H94" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="H94" s="30" t="s">
         <v>24</v>
       </c>
       <c r="I94" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="J94" s="32" t="s">
+      <c r="J94" s="30" t="s">
         <v>22</v>
       </c>
       <c r="K94" s="27">
         <v>0.71784665775934897</v>
       </c>
-      <c r="L94" s="34"/>
-      <c r="M94" s="34"/>
-      <c r="N94" s="34"/>
+      <c r="L94" s="32"/>
+      <c r="M94" s="32"/>
+      <c r="N94" s="32"/>
     </row>
     <row r="95" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B95" s="40"/>
+      <c r="B95" s="34"/>
       <c r="D95" s="33"/>
       <c r="E95" s="18"/>
       <c r="F95" s="18" t="s">
         <v>23</v>
       </c>
       <c r="G95" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="H95" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="H95" s="30" t="s">
         <v>24</v>
       </c>
       <c r="I95" s="25" t="s">
@@ -3514,21 +3520,21 @@
       <c r="K95" s="27">
         <v>68.430000000000007</v>
       </c>
-      <c r="L95" s="34"/>
-      <c r="M95" s="34"/>
-      <c r="N95" s="34"/>
+      <c r="L95" s="32"/>
+      <c r="M95" s="32"/>
+      <c r="N95" s="32"/>
     </row>
     <row r="96" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B96" s="40"/>
+      <c r="B96" s="34"/>
       <c r="D96" s="33"/>
       <c r="E96" s="18"/>
       <c r="F96" s="18" t="s">
         <v>25</v>
       </c>
       <c r="G96" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="H96" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="H96" s="30" t="s">
         <v>76</v>
       </c>
       <c r="I96" s="25" t="s">
@@ -3540,12 +3546,12 @@
       <c r="K96" s="27">
         <v>0.72422953987502703</v>
       </c>
-      <c r="L96" s="34"/>
-      <c r="M96" s="34"/>
-      <c r="N96" s="34"/>
+      <c r="L96" s="32"/>
+      <c r="M96" s="32"/>
+      <c r="N96" s="32"/>
     </row>
     <row r="97" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B97" s="40"/>
+      <c r="B97" s="34"/>
       <c r="D97" s="33"/>
       <c r="E97" s="18"/>
       <c r="F97" s="18" t="s">
@@ -3558,23 +3564,37 @@
       </c>
       <c r="J97" s="27"/>
       <c r="K97" s="27"/>
-      <c r="L97" s="34"/>
-      <c r="M97" s="34"/>
-      <c r="N97" s="34"/>
+      <c r="L97" s="32"/>
+      <c r="M97" s="32"/>
+      <c r="N97" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="N59:N65"/>
-    <mergeCell ref="M27:M33"/>
-    <mergeCell ref="M35:M41"/>
-    <mergeCell ref="M43:M49"/>
-    <mergeCell ref="M51:M57"/>
-    <mergeCell ref="M59:M65"/>
-    <mergeCell ref="M19:M25"/>
-    <mergeCell ref="N27:N33"/>
-    <mergeCell ref="N35:N41"/>
-    <mergeCell ref="N43:N49"/>
-    <mergeCell ref="N51:N57"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="D91:D97"/>
+    <mergeCell ref="L91:L97"/>
+    <mergeCell ref="M91:M97"/>
+    <mergeCell ref="N91:N97"/>
+    <mergeCell ref="D51:D57"/>
+    <mergeCell ref="D2:D9"/>
+    <mergeCell ref="D11:D17"/>
+    <mergeCell ref="D19:D25"/>
+    <mergeCell ref="D27:D33"/>
+    <mergeCell ref="D35:D41"/>
+    <mergeCell ref="N2:N9"/>
+    <mergeCell ref="N11:N17"/>
+    <mergeCell ref="N19:N25"/>
+    <mergeCell ref="M2:M9"/>
+    <mergeCell ref="M11:M17"/>
+    <mergeCell ref="B67:B97"/>
+    <mergeCell ref="D75:D81"/>
+    <mergeCell ref="L75:L81"/>
+    <mergeCell ref="M75:M81"/>
+    <mergeCell ref="N75:N81"/>
+    <mergeCell ref="D83:D89"/>
+    <mergeCell ref="L83:L89"/>
+    <mergeCell ref="M83:M89"/>
+    <mergeCell ref="N83:N89"/>
     <mergeCell ref="B2:B33"/>
     <mergeCell ref="D67:D73"/>
     <mergeCell ref="L67:L73"/>
@@ -3591,31 +3611,17 @@
     <mergeCell ref="L35:L41"/>
     <mergeCell ref="D59:D65"/>
     <mergeCell ref="D43:D49"/>
-    <mergeCell ref="B67:B97"/>
-    <mergeCell ref="D75:D81"/>
-    <mergeCell ref="L75:L81"/>
-    <mergeCell ref="M75:M81"/>
-    <mergeCell ref="N75:N81"/>
-    <mergeCell ref="D83:D89"/>
-    <mergeCell ref="L83:L89"/>
-    <mergeCell ref="M83:M89"/>
-    <mergeCell ref="N83:N89"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="D91:D97"/>
-    <mergeCell ref="L91:L97"/>
-    <mergeCell ref="M91:M97"/>
-    <mergeCell ref="N91:N97"/>
-    <mergeCell ref="D51:D57"/>
-    <mergeCell ref="D2:D9"/>
-    <mergeCell ref="D11:D17"/>
-    <mergeCell ref="D19:D25"/>
-    <mergeCell ref="D27:D33"/>
-    <mergeCell ref="D35:D41"/>
-    <mergeCell ref="N2:N9"/>
-    <mergeCell ref="N11:N17"/>
-    <mergeCell ref="N19:N25"/>
-    <mergeCell ref="M2:M9"/>
-    <mergeCell ref="M11:M17"/>
+    <mergeCell ref="M19:M25"/>
+    <mergeCell ref="N27:N33"/>
+    <mergeCell ref="N35:N41"/>
+    <mergeCell ref="N43:N49"/>
+    <mergeCell ref="N51:N57"/>
+    <mergeCell ref="N59:N65"/>
+    <mergeCell ref="M27:M33"/>
+    <mergeCell ref="M35:M41"/>
+    <mergeCell ref="M43:M49"/>
+    <mergeCell ref="M51:M57"/>
+    <mergeCell ref="M59:M65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>